<commit_message>
Persist table status & sync post_id
</commit_message>
<xml_diff>
--- a/Development Docs/ToDo.xlsx
+++ b/Development Docs/ToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greg\Local Sites\schaub-labs\app\public\wp-content\plugins\dynamic-tables\Development Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87045FDD-81DA-46F2-BC20-39C1F3298B5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9728CD8E-8612-4D6F-9BF9-7036F0ABFD00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="17520" xr2:uid="{A3DBE3D2-0DAF-4481-8DC4-68682F930EC6}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="93">
   <si>
     <t>Item</t>
   </si>
@@ -288,6 +288,36 @@
   </si>
   <si>
     <t>App, Store, Database</t>
+  </si>
+  <si>
+    <t>Delete table when post deleted from admin page</t>
+  </si>
+  <si>
+    <t>Job to remove orphan tables</t>
+  </si>
+  <si>
+    <t>Create admin page to maintain tables</t>
+  </si>
+  <si>
+    <t>Create table from CSV file</t>
+  </si>
+  <si>
+    <t>Determine if useEffect for # col/row is still needed</t>
+  </si>
+  <si>
+    <t>update edit.js to remove depricated useSetting</t>
+  </si>
+  <si>
+    <t>Remove red table border from block editor</t>
+  </si>
+  <si>
+    <t>Gray "Freeze  Header Row" when Headers are disabled</t>
+  </si>
+  <si>
+    <t>Remove the Site Save Message or make it meaningful</t>
+  </si>
+  <si>
+    <t>Testing</t>
   </si>
 </sst>
 </file>
@@ -660,16 +690,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9A95F50-2338-43A7-B2D8-210D78A54828}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:O52"/>
+  <dimension ref="A1:O61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.42578125" customWidth="1"/>
-    <col min="2" max="2" width="47.5703125" customWidth="1"/>
+    <col min="2" max="2" width="59.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.42578125" customWidth="1"/>
     <col min="4" max="4" width="27.140625" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" customWidth="1"/>
@@ -718,7 +748,7 @@
       <c r="N1" s="2"/>
       <c r="O1" s="3"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>14</v>
       </c>
@@ -744,7 +774,7 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -776,7 +806,7 @@
         <v>2</v>
       </c>
       <c r="J3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -808,7 +838,7 @@
         <v>3</v>
       </c>
       <c r="J4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -840,7 +870,7 @@
         <v>4</v>
       </c>
       <c r="J5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -901,7 +931,7 @@
         <v>6</v>
       </c>
       <c r="J7" t="s">
-        <v>27</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -2151,6 +2181,201 @@
       </c>
       <c r="J52" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>83</v>
+      </c>
+      <c r="C53" t="s">
+        <v>18</v>
+      </c>
+      <c r="E53" t="s">
+        <v>11</v>
+      </c>
+      <c r="F53" t="s">
+        <v>24</v>
+      </c>
+      <c r="J53" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>84</v>
+      </c>
+      <c r="C54" t="s">
+        <v>18</v>
+      </c>
+      <c r="E54" t="s">
+        <v>25</v>
+      </c>
+      <c r="F54" t="s">
+        <v>24</v>
+      </c>
+      <c r="J54" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>85</v>
+      </c>
+      <c r="C55" t="s">
+        <v>17</v>
+      </c>
+      <c r="E55" t="s">
+        <v>25</v>
+      </c>
+      <c r="F55" t="s">
+        <v>24</v>
+      </c>
+      <c r="G55">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J55" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>86</v>
+      </c>
+      <c r="C56" t="s">
+        <v>17</v>
+      </c>
+      <c r="E56" t="s">
+        <v>25</v>
+      </c>
+      <c r="F56" t="s">
+        <v>24</v>
+      </c>
+      <c r="G56">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J56" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>87</v>
+      </c>
+      <c r="C57" t="s">
+        <v>76</v>
+      </c>
+      <c r="D57" t="s">
+        <v>56</v>
+      </c>
+      <c r="E57" t="s">
+        <v>6</v>
+      </c>
+      <c r="F57" t="s">
+        <v>7</v>
+      </c>
+      <c r="G57">
+        <v>1</v>
+      </c>
+      <c r="J57" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>88</v>
+      </c>
+      <c r="C58" t="s">
+        <v>76</v>
+      </c>
+      <c r="D58" t="s">
+        <v>56</v>
+      </c>
+      <c r="E58" t="s">
+        <v>6</v>
+      </c>
+      <c r="F58" t="s">
+        <v>7</v>
+      </c>
+      <c r="G58">
+        <v>1</v>
+      </c>
+      <c r="J58" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>89</v>
+      </c>
+      <c r="C59" t="s">
+        <v>76</v>
+      </c>
+      <c r="D59" t="s">
+        <v>56</v>
+      </c>
+      <c r="E59" t="s">
+        <v>6</v>
+      </c>
+      <c r="F59" t="s">
+        <v>7</v>
+      </c>
+      <c r="G59">
+        <v>1</v>
+      </c>
+      <c r="J59" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>90</v>
+      </c>
+      <c r="C60" t="s">
+        <v>76</v>
+      </c>
+      <c r="D60" t="s">
+        <v>56</v>
+      </c>
+      <c r="E60" t="s">
+        <v>6</v>
+      </c>
+      <c r="F60" t="s">
+        <v>7</v>
+      </c>
+      <c r="G60">
+        <v>1</v>
+      </c>
+      <c r="J60" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Move banded rows from row-cells to rows
</commit_message>
<xml_diff>
--- a/Development Docs/ToDo.xlsx
+++ b/Development Docs/ToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greg\Local Sites\schaub-labs\app\public\wp-content\plugins\dynamic-tables\Development Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9728CD8E-8612-4D6F-9BF9-7036F0ABFD00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D53285C4-9FE4-4991-8899-5EC5571A5D52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="17520" xr2:uid="{A3DBE3D2-0DAF-4481-8DC4-68682F930EC6}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$K$52</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$K$62</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="95">
   <si>
     <t>Item</t>
   </si>
@@ -318,6 +318,12 @@
   </si>
   <si>
     <t>Testing</t>
+  </si>
+  <si>
+    <t>Enable undo functionality</t>
+  </si>
+  <si>
+    <t>UX</t>
   </si>
 </sst>
 </file>
@@ -365,7 +371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -375,6 +381,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -690,10 +697,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9A95F50-2338-43A7-B2D8-210D78A54828}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:O61"/>
+  <dimension ref="A1:O62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,14 +777,11 @@
       <c r="G2">
         <v>1</v>
       </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
       <c r="J2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>15</v>
       </c>
@@ -799,17 +803,11 @@
       <c r="G3">
         <v>1</v>
       </c>
-      <c r="H3" s="4">
-        <v>14</v>
-      </c>
-      <c r="I3">
-        <v>2</v>
-      </c>
       <c r="J3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>16</v>
       </c>
@@ -831,17 +829,11 @@
       <c r="G4">
         <v>1</v>
       </c>
-      <c r="H4" s="4">
-        <v>14</v>
-      </c>
-      <c r="I4">
-        <v>3</v>
-      </c>
       <c r="J4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>17</v>
       </c>
@@ -863,17 +855,11 @@
       <c r="G5">
         <v>1</v>
       </c>
-      <c r="H5" s="4">
-        <v>15</v>
-      </c>
-      <c r="I5">
-        <v>4</v>
-      </c>
       <c r="J5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>51</v>
       </c>
@@ -895,11 +881,8 @@
       <c r="G6">
         <v>1</v>
       </c>
-      <c r="I6">
-        <v>5</v>
-      </c>
       <c r="J6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -928,7 +911,7 @@
         <v>17</v>
       </c>
       <c r="I7">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="J7" t="s">
         <v>92</v>
@@ -957,7 +940,7 @@
         <v>1</v>
       </c>
       <c r="I8">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="J8" t="s">
         <v>27</v>
@@ -986,7 +969,7 @@
         <v>1</v>
       </c>
       <c r="I9">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="J9" t="s">
         <v>27</v>
@@ -1015,7 +998,7 @@
         <v>1</v>
       </c>
       <c r="I10">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="J10" t="s">
         <v>27</v>
@@ -1047,7 +1030,7 @@
         <v>32</v>
       </c>
       <c r="I11">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="J11" t="s">
         <v>27</v>
@@ -1076,7 +1059,7 @@
         <v>1</v>
       </c>
       <c r="I12">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="J12" t="s">
         <v>27</v>
@@ -1105,7 +1088,7 @@
         <v>1</v>
       </c>
       <c r="I13">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="J13" t="s">
         <v>27</v>
@@ -1134,7 +1117,7 @@
         <v>1</v>
       </c>
       <c r="I14">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="J14" t="s">
         <v>27</v>
@@ -1163,7 +1146,7 @@
         <v>1</v>
       </c>
       <c r="I15">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="J15" t="s">
         <v>27</v>
@@ -1192,7 +1175,7 @@
         <v>1</v>
       </c>
       <c r="I16">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="J16" t="s">
         <v>27</v>
@@ -1200,13 +1183,13 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="B17" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="C17" t="s">
-        <v>17</v>
+        <v>94</v>
       </c>
       <c r="D17" t="s">
         <v>56</v>
@@ -1221,7 +1204,7 @@
         <v>1</v>
       </c>
       <c r="I17">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="J17" t="s">
         <v>27</v>
@@ -1229,19 +1212,19 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>90</v>
       </c>
       <c r="C18" t="s">
-        <v>18</v>
+        <v>76</v>
       </c>
       <c r="D18" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="E18" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F18" t="s">
         <v>7</v>
@@ -1250,7 +1233,7 @@
         <v>1</v>
       </c>
       <c r="I18">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="J18" t="s">
         <v>27</v>
@@ -1258,10 +1241,10 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B19" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C19" t="s">
         <v>17</v>
@@ -1270,7 +1253,7 @@
         <v>56</v>
       </c>
       <c r="E19" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F19" t="s">
         <v>7</v>
@@ -1279,7 +1262,7 @@
         <v>1</v>
       </c>
       <c r="I19">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="J19" t="s">
         <v>27</v>
@@ -1287,19 +1270,19 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B20" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="C20" t="s">
         <v>18</v>
       </c>
       <c r="D20" t="s">
-        <v>75</v>
+        <v>31</v>
       </c>
       <c r="E20" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F20" t="s">
         <v>7</v>
@@ -1307,11 +1290,8 @@
       <c r="G20">
         <v>1</v>
       </c>
-      <c r="H20" s="4" t="s">
-        <v>80</v>
-      </c>
       <c r="I20">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="J20" t="s">
         <v>27</v>
@@ -1319,16 +1299,16 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B21" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D21" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="E21" t="s">
         <v>11</v>
@@ -1340,7 +1320,7 @@
         <v>1</v>
       </c>
       <c r="I21">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="J21" t="s">
         <v>27</v>
@@ -1348,19 +1328,19 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="B22" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="C22" t="s">
-        <v>18</v>
+        <v>76</v>
       </c>
       <c r="D22" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="E22" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F22" t="s">
         <v>7</v>
@@ -1369,7 +1349,7 @@
         <v>1</v>
       </c>
       <c r="I22">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="J22" t="s">
         <v>27</v>
@@ -1377,10 +1357,10 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="B23" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="C23" t="s">
         <v>76</v>
@@ -1389,7 +1369,7 @@
         <v>56</v>
       </c>
       <c r="E23" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="F23" t="s">
         <v>7</v>
@@ -1398,7 +1378,7 @@
         <v>1</v>
       </c>
       <c r="I23">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="J23" t="s">
         <v>27</v>
@@ -1406,19 +1386,19 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="B24" t="s">
-        <v>69</v>
+        <v>91</v>
       </c>
       <c r="C24" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="D24" t="s">
         <v>56</v>
       </c>
       <c r="E24" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="F24" t="s">
         <v>7</v>
@@ -1427,7 +1407,7 @@
         <v>1</v>
       </c>
       <c r="I24">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="J24" t="s">
         <v>27</v>
@@ -2078,7 +2058,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>37</v>
       </c>
@@ -2105,133 +2085,167 @@
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="B50" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
       <c r="C50" t="s">
         <v>18</v>
       </c>
       <c r="D50" t="s">
-        <v>21</v>
+        <v>75</v>
       </c>
       <c r="E50" t="s">
         <v>25</v>
       </c>
       <c r="F50" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="G50">
-        <v>1.1000000000000001</v>
+        <v>1</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="I50">
+        <v>19</v>
       </c>
       <c r="J50" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K50" s="5"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="B51" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="C51" t="s">
         <v>18</v>
       </c>
       <c r="D51" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
       <c r="E51" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="F51" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="G51">
-        <v>1.1000000000000001</v>
+        <v>1</v>
+      </c>
+      <c r="I51">
+        <v>20</v>
       </c>
       <c r="J51" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="B52" t="s">
+        <v>64</v>
+      </c>
+      <c r="C52" t="s">
+        <v>18</v>
+      </c>
+      <c r="D52" t="s">
+        <v>75</v>
+      </c>
+      <c r="E52" t="s">
+        <v>11</v>
+      </c>
+      <c r="F52" t="s">
+        <v>7</v>
+      </c>
+      <c r="G52">
+        <v>1</v>
+      </c>
+      <c r="I52">
+        <v>21</v>
+      </c>
+      <c r="J52" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>44</v>
+      </c>
+      <c r="B53" t="s">
+        <v>68</v>
+      </c>
+      <c r="C53" t="s">
+        <v>76</v>
+      </c>
+      <c r="D53" t="s">
+        <v>56</v>
+      </c>
+      <c r="E53" t="s">
+        <v>25</v>
+      </c>
+      <c r="F53" t="s">
+        <v>7</v>
+      </c>
+      <c r="G53">
+        <v>1</v>
+      </c>
+      <c r="I53">
         <v>22</v>
       </c>
-      <c r="C52" t="s">
-        <v>17</v>
-      </c>
-      <c r="D52" t="s">
-        <v>20</v>
-      </c>
-      <c r="E52" t="s">
-        <v>25</v>
-      </c>
-      <c r="F52" t="s">
-        <v>24</v>
-      </c>
-      <c r="G52">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="J52" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>52</v>
-      </c>
-      <c r="B53" t="s">
-        <v>83</v>
-      </c>
-      <c r="C53" t="s">
-        <v>18</v>
-      </c>
-      <c r="E53" t="s">
-        <v>11</v>
-      </c>
-      <c r="F53" t="s">
-        <v>24</v>
-      </c>
       <c r="J53" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B54" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="C54" t="s">
-        <v>18</v>
+        <v>76</v>
+      </c>
+      <c r="D54" t="s">
+        <v>56</v>
       </c>
       <c r="E54" t="s">
         <v>25</v>
       </c>
       <c r="F54" t="s">
-        <v>24</v>
+        <v>7</v>
+      </c>
+      <c r="G54">
+        <v>1</v>
+      </c>
+      <c r="I54">
+        <v>23</v>
       </c>
       <c r="J54" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="B55" t="s">
-        <v>85</v>
+        <v>35</v>
       </c>
       <c r="C55" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="D55" t="s">
+        <v>21</v>
       </c>
       <c r="E55" t="s">
         <v>25</v>
@@ -2246,18 +2260,21 @@
         <v>27</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="B56" t="s">
-        <v>86</v>
+        <v>30</v>
       </c>
       <c r="C56" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="D56" t="s">
+        <v>31</v>
       </c>
       <c r="E56" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="F56" t="s">
         <v>24</v>
@@ -2269,130 +2286,160 @@
         <v>27</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="B57" t="s">
-        <v>87</v>
+        <v>22</v>
       </c>
       <c r="C57" t="s">
-        <v>76</v>
+        <v>17</v>
       </c>
       <c r="D57" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="E57" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="F57" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="G57">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J57" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B58" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C58" t="s">
-        <v>76</v>
-      </c>
-      <c r="D58" t="s">
-        <v>56</v>
+        <v>17</v>
       </c>
       <c r="E58" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="F58" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="G58">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J58" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B59" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C59" t="s">
-        <v>76</v>
-      </c>
-      <c r="D59" t="s">
-        <v>56</v>
+        <v>17</v>
       </c>
       <c r="E59" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="F59" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="G59">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J59" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B60" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C60" t="s">
-        <v>76</v>
+        <v>17</v>
       </c>
       <c r="D60" t="s">
         <v>56</v>
       </c>
       <c r="E60" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="F60" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G60">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J60" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>52</v>
+      </c>
       <c r="B61" t="s">
-        <v>91</v>
+        <v>83</v>
+      </c>
+      <c r="C61" t="s">
+        <v>18</v>
+      </c>
+      <c r="E61" t="s">
+        <v>11</v>
+      </c>
+      <c r="F61" t="s">
+        <v>24</v>
+      </c>
+      <c r="J61" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>53</v>
+      </c>
+      <c r="B62" t="s">
+        <v>84</v>
+      </c>
+      <c r="C62" t="s">
+        <v>18</v>
+      </c>
+      <c r="E62" t="s">
+        <v>25</v>
+      </c>
+      <c r="F62" t="s">
+        <v>24</v>
+      </c>
+      <c r="J62" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:K52" xr:uid="{C9A95F50-2338-43A7-B2D8-210D78A54828}">
+  <autoFilter ref="B1:K62" xr:uid="{C9A95F50-2338-43A7-B2D8-210D78A54828}">
     <filterColumn colId="8">
       <filters>
         <filter val="Open"/>
+        <filter val="Testing"/>
       </filters>
     </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:K37">
       <sortCondition ref="I2:I37"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K66">
-    <sortCondition ref="G2:G66"/>
-    <sortCondition ref="I2:I66"/>
-    <sortCondition ref="A2:A66"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:K62">
+    <sortCondition ref="G2:G62"/>
+    <sortCondition ref="I2:I62"/>
+    <sortCondition ref="A2:A62"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Disable Sticky Header when Header not present
</commit_message>
<xml_diff>
--- a/Development Docs/ToDo.xlsx
+++ b/Development Docs/ToDo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greg\Local Sites\schaub-labs\app\public\wp-content\plugins\dynamic-tables\Development Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D53285C4-9FE4-4991-8899-5EC5571A5D52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F940C9BC-C8FB-41F0-919E-C159CD0FDE37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="17520" xr2:uid="{A3DBE3D2-0DAF-4481-8DC4-68682F930EC6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{A3DBE3D2-0DAF-4481-8DC4-68682F930EC6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="96">
   <si>
     <t>Item</t>
   </si>
@@ -324,6 +324,9 @@
   </si>
   <si>
     <t>UX</t>
+  </si>
+  <si>
+    <t>Researching</t>
   </si>
 </sst>
 </file>
@@ -700,7 +703,7 @@
   <dimension ref="A1:O62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,7 +717,7 @@
     <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.28515625" style="4" customWidth="1"/>
     <col min="9" max="9" width="7.85546875" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="45.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -943,7 +946,7 @@
         <v>2</v>
       </c>
       <c r="J8" t="s">
-        <v>27</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -1120,7 +1123,7 @@
         <v>8</v>
       </c>
       <c r="J14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Get Security and split Web Service php
</commit_message>
<xml_diff>
--- a/Development Docs/ToDo.xlsx
+++ b/Development Docs/ToDo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greg\Local Sites\schaub-labs\app\public\wp-content\plugins\dynamic-tables\Development Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B99C859-6D1B-449D-B09A-38DD414A9A33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3429C2A-9A10-4C02-A749-4CFED26CD98C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="16470" xr2:uid="{A3DBE3D2-0DAF-4481-8DC4-68682F930EC6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="17520" xr2:uid="{A3DBE3D2-0DAF-4481-8DC4-68682F930EC6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="101">
   <si>
     <t>Item</t>
   </si>
@@ -326,9 +326,6 @@
     <t>UX</t>
   </si>
   <si>
-    <t>Researching</t>
-  </si>
-  <si>
     <t>Optionally show/hide title</t>
   </si>
   <si>
@@ -339,6 +336,12 @@
   </si>
   <si>
     <t>Replace Drop Down Menu to V2</t>
+  </si>
+  <si>
+    <t>Hold</t>
+  </si>
+  <si>
+    <t>Nonces are handled automatically by Gutenberg and the Rest API for block editor.  There will be a need when frontend editing is enabled.</t>
   </si>
 </sst>
 </file>
@@ -394,18 +397,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -724,60 +739,60 @@
   <dimension ref="A1:O66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" customWidth="1"/>
-    <col min="2" max="2" width="59.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="45.5703125" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="59.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" style="6" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" style="5" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="64.28515625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="N1" s="2"/>
-      <c r="O1" s="3"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="10"/>
     </row>
     <row r="2" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -801,9 +816,12 @@
       <c r="G2">
         <v>1</v>
       </c>
+      <c r="H2" s="1"/>
+      <c r="I2"/>
       <c r="J2" t="s">
         <v>26</v>
       </c>
+      <c r="K2"/>
     </row>
     <row r="3" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -827,9 +845,12 @@
       <c r="G3">
         <v>1</v>
       </c>
+      <c r="H3" s="1"/>
+      <c r="I3"/>
       <c r="J3" t="s">
         <v>26</v>
       </c>
+      <c r="K3"/>
     </row>
     <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -853,9 +874,12 @@
       <c r="G4">
         <v>1</v>
       </c>
+      <c r="H4" s="1"/>
+      <c r="I4"/>
       <c r="J4" t="s">
         <v>26</v>
       </c>
+      <c r="K4"/>
     </row>
     <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -879,9 +903,12 @@
       <c r="G5">
         <v>1</v>
       </c>
+      <c r="H5" s="1"/>
+      <c r="I5"/>
       <c r="J5" t="s">
         <v>26</v>
       </c>
+      <c r="K5"/>
     </row>
     <row r="6" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -905,187 +932,190 @@
       <c r="G6">
         <v>1</v>
       </c>
+      <c r="H6" s="1"/>
+      <c r="I6"/>
       <c r="J6" t="s">
         <v>26</v>
       </c>
+      <c r="K6"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="5">
         <v>49</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7" s="4">
+      <c r="F7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="5">
+        <v>1</v>
+      </c>
+      <c r="H7" s="6">
         <v>17</v>
       </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-      <c r="J7" t="s">
+      <c r="I7" s="5">
+        <v>1</v>
+      </c>
+      <c r="J7" s="5" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
         <v>32</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="C8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="E8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="G8" s="5">
+        <v>1</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>33</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="I8">
-        <v>2</v>
-      </c>
-      <c r="J8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>33</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="G9" s="5">
+        <v>1</v>
+      </c>
+      <c r="I9" s="5">
+        <v>3</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>34</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="5">
+        <v>1</v>
+      </c>
+      <c r="I10" s="5">
+        <v>4</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>50</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="5">
+        <v>1</v>
+      </c>
+      <c r="H11" s="6">
         <v>32</v>
       </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="I11" s="5">
+        <v>5</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>35</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="I9">
-        <v>3</v>
-      </c>
-      <c r="J9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>34</v>
-      </c>
-      <c r="B10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" t="s">
-        <v>6</v>
-      </c>
-      <c r="F10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="I10">
-        <v>4</v>
-      </c>
-      <c r="J10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>50</v>
-      </c>
-      <c r="B11" t="s">
-        <v>77</v>
-      </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" t="s">
-        <v>7</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11" s="4">
-        <v>32</v>
-      </c>
-      <c r="I11">
-        <v>5</v>
-      </c>
-      <c r="J11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>35</v>
-      </c>
-      <c r="B12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" t="s">
-        <v>6</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="E12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="I12">
-        <v>6</v>
-      </c>
-      <c r="J12" t="s">
+      <c r="G12" s="5">
+        <v>1</v>
+      </c>
+      <c r="I12" s="5">
+        <v>6</v>
+      </c>
+      <c r="J12" s="5" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1111,9 +1141,12 @@
       <c r="G13">
         <v>1</v>
       </c>
-      <c r="J13" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="H13" s="1"/>
+      <c r="I13"/>
+      <c r="J13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K13"/>
     </row>
     <row r="14" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -1137,94 +1170,97 @@
       <c r="G14">
         <v>1</v>
       </c>
-      <c r="J14" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="H14" s="1"/>
+      <c r="I14"/>
+      <c r="J14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K14"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="5">
         <v>46</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E15" t="s">
-        <v>6</v>
-      </c>
-      <c r="F15" t="s">
-        <v>7</v>
-      </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-      <c r="I15">
+      <c r="E15" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" s="5">
+        <v>1</v>
+      </c>
+      <c r="I15" s="5">
         <v>9</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J15" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="5">
         <v>47</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E16" t="s">
-        <v>6</v>
-      </c>
-      <c r="F16" t="s">
-        <v>7</v>
-      </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
-      <c r="I16">
+      <c r="E16" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" s="5">
+        <v>1</v>
+      </c>
+      <c r="I16" s="5">
         <v>10</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J16" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="A17" s="5">
         <v>58</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E17" t="s">
-        <v>6</v>
-      </c>
-      <c r="F17" t="s">
-        <v>7</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-      <c r="I17">
+      <c r="E17" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" s="5">
+        <v>1</v>
+      </c>
+      <c r="I17" s="5">
         <v>11</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J17" s="5" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1250,9 +1286,12 @@
       <c r="G18">
         <v>1</v>
       </c>
-      <c r="J18" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="H18" s="1"/>
+      <c r="I18"/>
+      <c r="J18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K18"/>
     </row>
     <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
@@ -1276,152 +1315,155 @@
       <c r="G19">
         <v>1</v>
       </c>
-      <c r="J19" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="H19" s="1"/>
+      <c r="I19"/>
+      <c r="J19" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K19"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="A20" s="5">
         <v>62</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" s="5">
+        <v>1</v>
+      </c>
+      <c r="I20" s="5">
+        <v>14</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>63</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D21" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E20" t="s">
-        <v>6</v>
-      </c>
-      <c r="F20" t="s">
-        <v>7</v>
-      </c>
-      <c r="G20">
-        <v>1</v>
-      </c>
-      <c r="I20">
-        <v>14</v>
-      </c>
-      <c r="J20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>63</v>
-      </c>
-      <c r="B21" t="s">
-        <v>97</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="E21" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" s="5">
+        <v>1</v>
+      </c>
+      <c r="I21" s="5">
+        <v>15</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>36</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" s="5">
+        <v>1</v>
+      </c>
+      <c r="I22" s="5">
+        <v>16</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>43</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D23" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E21" t="s">
-        <v>6</v>
-      </c>
-      <c r="F21" t="s">
-        <v>7</v>
-      </c>
-      <c r="G21">
-        <v>1</v>
-      </c>
-      <c r="I21">
-        <v>15</v>
-      </c>
-      <c r="J21" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>36</v>
-      </c>
-      <c r="B22" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" t="s">
-        <v>31</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="E23" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F22" t="s">
-        <v>7</v>
-      </c>
-      <c r="G22">
-        <v>1</v>
-      </c>
-      <c r="I22">
-        <v>16</v>
-      </c>
-      <c r="J22" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>43</v>
-      </c>
-      <c r="B23" t="s">
-        <v>67</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="F23" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23" s="5">
+        <v>1</v>
+      </c>
+      <c r="I23" s="5">
         <v>17</v>
       </c>
-      <c r="D23" t="s">
+      <c r="J23" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
         <v>56</v>
       </c>
-      <c r="E23" t="s">
-        <v>11</v>
-      </c>
-      <c r="F23" t="s">
-        <v>7</v>
-      </c>
-      <c r="G23">
-        <v>1</v>
-      </c>
-      <c r="I23">
-        <v>17</v>
-      </c>
-      <c r="J23" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="B24" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B24" t="s">
-        <v>87</v>
-      </c>
-      <c r="C24" t="s">
-        <v>76</v>
-      </c>
-      <c r="D24" t="s">
-        <v>56</v>
-      </c>
-      <c r="E24" t="s">
-        <v>6</v>
-      </c>
-      <c r="F24" t="s">
-        <v>7</v>
-      </c>
-      <c r="G24">
-        <v>1</v>
-      </c>
-      <c r="I24">
-        <v>18</v>
-      </c>
-      <c r="J24" t="s">
+      <c r="E24" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" s="5">
+        <v>1</v>
+      </c>
+      <c r="I24" s="5">
+        <v>18</v>
+      </c>
+      <c r="J24" s="5" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1448,6 +1490,7 @@
         <v>1</v>
       </c>
       <c r="H25"/>
+      <c r="I25"/>
       <c r="J25" t="s">
         <v>26</v>
       </c>
@@ -1478,6 +1521,7 @@
         <v>1</v>
       </c>
       <c r="H26"/>
+      <c r="I26"/>
       <c r="J26" t="s">
         <v>26</v>
       </c>
@@ -1508,6 +1552,7 @@
         <v>1</v>
       </c>
       <c r="H27"/>
+      <c r="I27"/>
       <c r="J27" t="s">
         <v>26</v>
       </c>
@@ -1538,6 +1583,7 @@
         <v>1</v>
       </c>
       <c r="H28"/>
+      <c r="I28"/>
       <c r="J28" t="s">
         <v>26</v>
       </c>
@@ -1568,6 +1614,7 @@
         <v>1</v>
       </c>
       <c r="H29"/>
+      <c r="I29"/>
       <c r="J29" t="s">
         <v>26</v>
       </c>
@@ -1598,6 +1645,7 @@
         <v>1</v>
       </c>
       <c r="H30"/>
+      <c r="I30"/>
       <c r="J30" t="s">
         <v>26</v>
       </c>
@@ -1628,9 +1676,11 @@
         <v>1</v>
       </c>
       <c r="H31"/>
+      <c r="I31"/>
       <c r="J31" t="s">
         <v>26</v>
       </c>
+      <c r="K31"/>
     </row>
     <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32">
@@ -1655,11 +1705,13 @@
         <v>1</v>
       </c>
       <c r="H32"/>
+      <c r="I32"/>
       <c r="J32" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="K32"/>
+    </row>
+    <row r="33" spans="1:10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>9</v>
       </c>
@@ -1681,12 +1733,11 @@
       <c r="G33">
         <v>1</v>
       </c>
-      <c r="H33"/>
       <c r="J33" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>10</v>
       </c>
@@ -1708,12 +1759,11 @@
       <c r="G34">
         <v>1</v>
       </c>
-      <c r="H34"/>
       <c r="J34" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>11</v>
       </c>
@@ -1735,12 +1785,11 @@
       <c r="G35">
         <v>1</v>
       </c>
-      <c r="H35"/>
       <c r="J35" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>12</v>
       </c>
@@ -1762,12 +1811,11 @@
       <c r="G36">
         <v>1</v>
       </c>
-      <c r="H36"/>
       <c r="J36" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>13</v>
       </c>
@@ -1789,12 +1837,11 @@
       <c r="G37">
         <v>1</v>
       </c>
-      <c r="H37"/>
       <c r="J37" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>18</v>
       </c>
@@ -1816,12 +1863,11 @@
       <c r="G38">
         <v>1</v>
       </c>
-      <c r="H38"/>
       <c r="J38" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>19</v>
       </c>
@@ -1843,12 +1889,11 @@
       <c r="G39">
         <v>1</v>
       </c>
-      <c r="H39"/>
       <c r="J39" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>20</v>
       </c>
@@ -1870,12 +1915,11 @@
       <c r="G40">
         <v>1</v>
       </c>
-      <c r="H40"/>
       <c r="J40" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>21</v>
       </c>
@@ -1897,12 +1941,11 @@
       <c r="G41">
         <v>1</v>
       </c>
-      <c r="H41"/>
       <c r="J41" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>22</v>
       </c>
@@ -1924,12 +1967,11 @@
       <c r="G42">
         <v>1</v>
       </c>
-      <c r="H42"/>
       <c r="J42" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>23</v>
       </c>
@@ -1951,12 +1993,11 @@
       <c r="G43">
         <v>1</v>
       </c>
-      <c r="H43"/>
       <c r="J43" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>24</v>
       </c>
@@ -1978,12 +2019,11 @@
       <c r="G44">
         <v>1</v>
       </c>
-      <c r="H44"/>
       <c r="J44" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>25</v>
       </c>
@@ -2005,12 +2045,11 @@
       <c r="G45">
         <v>1</v>
       </c>
-      <c r="H45"/>
       <c r="J45" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>27</v>
       </c>
@@ -2032,12 +2071,11 @@
       <c r="G46">
         <v>1</v>
       </c>
-      <c r="H46"/>
       <c r="J46" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>28</v>
       </c>
@@ -2059,12 +2097,11 @@
       <c r="G47">
         <v>1</v>
       </c>
-      <c r="H47"/>
       <c r="J47" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>30</v>
       </c>
@@ -2083,7 +2120,6 @@
       <c r="G48">
         <v>1</v>
       </c>
-      <c r="H48"/>
       <c r="J48" t="s">
         <v>26</v>
       </c>
@@ -2111,462 +2147,464 @@
         <v>1</v>
       </c>
       <c r="H49"/>
+      <c r="I49"/>
       <c r="J49" t="s">
         <v>26</v>
       </c>
+      <c r="K49"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50">
+      <c r="A50" s="5">
         <v>57</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E50" t="s">
-        <v>6</v>
-      </c>
-      <c r="F50" t="s">
-        <v>7</v>
-      </c>
-      <c r="G50">
-        <v>1</v>
-      </c>
-      <c r="I50">
+      <c r="E50" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G50" s="5">
+        <v>1</v>
+      </c>
+      <c r="I50" s="5">
         <v>19</v>
       </c>
-      <c r="J50" t="s">
+      <c r="J50" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51">
+      <c r="A51" s="5">
         <v>60</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E51" t="s">
-        <v>6</v>
-      </c>
-      <c r="F51" t="s">
-        <v>7</v>
-      </c>
-      <c r="G51">
-        <v>1</v>
-      </c>
-      <c r="I51">
+      <c r="E51" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G51" s="5">
+        <v>1</v>
+      </c>
+      <c r="I51" s="5">
         <v>20</v>
       </c>
-      <c r="J51" t="s">
+      <c r="J51" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52">
+      <c r="A52" s="5">
         <v>38</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C52" t="s">
-        <v>18</v>
-      </c>
-      <c r="D52" t="s">
+      <c r="C52" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D52" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E52" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F52" t="s">
-        <v>7</v>
-      </c>
-      <c r="G52">
-        <v>1</v>
-      </c>
-      <c r="H52" s="4" t="s">
+      <c r="F52" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G52" s="5">
+        <v>1</v>
+      </c>
+      <c r="H52" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="I52">
+      <c r="I52" s="5">
         <v>21</v>
       </c>
-      <c r="J52" t="s">
-        <v>27</v>
-      </c>
-      <c r="K52" s="5"/>
+      <c r="J52" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K52" s="7"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53">
+      <c r="A53" s="5">
         <v>39</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C53" t="s">
-        <v>18</v>
-      </c>
-      <c r="D53" t="s">
+      <c r="C53" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D53" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E53" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F53" t="s">
-        <v>7</v>
-      </c>
-      <c r="G53">
-        <v>1</v>
-      </c>
-      <c r="I53">
+      <c r="F53" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G53" s="5">
+        <v>1</v>
+      </c>
+      <c r="I53" s="5">
         <v>22</v>
       </c>
-      <c r="J53" t="s">
+      <c r="J53" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54">
+      <c r="A54" s="5">
         <v>40</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C54" t="s">
-        <v>18</v>
-      </c>
-      <c r="D54" t="s">
+      <c r="C54" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D54" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E54" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F54" t="s">
-        <v>7</v>
-      </c>
-      <c r="G54">
-        <v>1</v>
-      </c>
-      <c r="I54">
+      <c r="F54" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G54" s="5">
+        <v>1</v>
+      </c>
+      <c r="I54" s="5">
         <v>23</v>
       </c>
-      <c r="J54" t="s">
+      <c r="J54" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55">
+      <c r="A55" s="5">
         <v>44</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D55" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E55" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F55" t="s">
-        <v>7</v>
-      </c>
-      <c r="G55">
-        <v>1</v>
-      </c>
-      <c r="I55">
+      <c r="F55" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G55" s="5">
+        <v>1</v>
+      </c>
+      <c r="I55" s="5">
         <v>24</v>
       </c>
-      <c r="J55" t="s">
+      <c r="J55" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56">
+      <c r="A56" s="5">
         <v>45</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D56" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E56" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F56" t="s">
-        <v>7</v>
-      </c>
-      <c r="G56">
-        <v>1</v>
-      </c>
-      <c r="I56">
+      <c r="F56" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G56" s="5">
+        <v>1</v>
+      </c>
+      <c r="I56" s="5">
         <v>25</v>
       </c>
-      <c r="J56" t="s">
+      <c r="J56" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>26</v>
-      </c>
-      <c r="B57" t="s">
+      <c r="A57" s="5">
+        <v>26</v>
+      </c>
+      <c r="B57" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C57" t="s">
-        <v>18</v>
-      </c>
-      <c r="D57" t="s">
+      <c r="C57" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D57" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E57" t="s">
+      <c r="E57" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F57" t="s">
+      <c r="F57" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G57">
+      <c r="G57" s="5">
         <v>1.1000000000000001</v>
       </c>
-      <c r="J57" t="s">
+      <c r="J57" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58">
+      <c r="A58" s="5">
         <v>29</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C58" t="s">
-        <v>18</v>
-      </c>
-      <c r="D58" t="s">
+      <c r="C58" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D58" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E58" t="s">
-        <v>6</v>
-      </c>
-      <c r="F58" t="s">
+      <c r="E58" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F58" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G58">
+      <c r="G58" s="5">
         <v>1.1000000000000001</v>
       </c>
-      <c r="J58" t="s">
+      <c r="J58" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59">
+      <c r="A59" s="5">
         <v>31</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D59" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E59" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F59" t="s">
+      <c r="F59" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G59">
+      <c r="G59" s="5">
         <v>1.1000000000000001</v>
       </c>
-      <c r="J59" t="s">
+      <c r="J59" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60">
+      <c r="A60" s="5">
         <v>52</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C60" t="s">
-        <v>18</v>
-      </c>
-      <c r="E60" t="s">
+      <c r="C60" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E60" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F60" t="s">
+      <c r="F60" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G60">
+      <c r="G60" s="5">
         <v>1.1000000000000001</v>
       </c>
-      <c r="J60" t="s">
+      <c r="J60" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A61">
+      <c r="A61" s="5">
         <v>53</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C61" t="s">
-        <v>18</v>
-      </c>
-      <c r="E61" t="s">
+      <c r="C61" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E61" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F61" t="s">
+      <c r="F61" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G61">
+      <c r="G61" s="5">
         <v>1.1000000000000001</v>
       </c>
-      <c r="J61" t="s">
+      <c r="J61" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A62">
+      <c r="A62" s="5">
         <v>54</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E62" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F62" t="s">
+      <c r="F62" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G62">
+      <c r="G62" s="5">
         <v>1.1000000000000001</v>
       </c>
-      <c r="J62" t="s">
+      <c r="J62" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A63">
+      <c r="A63" s="5">
         <v>55</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E63" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F63" t="s">
+      <c r="F63" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G63">
+      <c r="G63" s="5">
         <v>1.1000000000000001</v>
       </c>
-      <c r="J63" t="s">
+      <c r="J63" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A64">
+      <c r="A64" s="5">
         <v>61</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D64" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E64" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F64" t="s">
+      <c r="F64" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G64">
+      <c r="G64" s="5">
         <v>1.1000000000000001</v>
       </c>
-      <c r="J64" t="s">
+      <c r="J64" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A65">
+      <c r="A65" s="5">
         <v>64</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G65" s="5">
+        <v>1</v>
+      </c>
+      <c r="J65" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66" s="5">
+        <v>65</v>
+      </c>
+      <c r="B66" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C65" t="s">
-        <v>76</v>
-      </c>
-      <c r="D65" t="s">
+      <c r="C66" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D66" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E65" t="s">
-        <v>6</v>
-      </c>
-      <c r="F65" t="s">
-        <v>7</v>
-      </c>
-      <c r="G65">
-        <v>1</v>
-      </c>
-      <c r="J65" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <v>65</v>
-      </c>
-      <c r="B66" t="s">
-        <v>99</v>
-      </c>
-      <c r="C66" t="s">
-        <v>94</v>
-      </c>
-      <c r="D66" t="s">
-        <v>56</v>
-      </c>
-      <c r="E66" t="s">
-        <v>6</v>
-      </c>
-      <c r="F66" t="s">
+      <c r="E66" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F66" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G66">
+      <c r="G66" s="5">
         <v>1.1000000000000001</v>
       </c>
-      <c r="J66" t="s">
+      <c r="J66" s="5" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updt DB on activate/Uninst. Option hide title
</commit_message>
<xml_diff>
--- a/Development Docs/ToDo.xlsx
+++ b/Development Docs/ToDo.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greg\Local Sites\schaub-labs\app\public\wp-content\plugins\dynamic-tables\Development Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3429C2A-9A10-4C02-A749-4CFED26CD98C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{720200F6-2116-47EE-A2A4-EFD9F0D7C7CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="17520" xr2:uid="{A3DBE3D2-0DAF-4481-8DC4-68682F930EC6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{A3DBE3D2-0DAF-4481-8DC4-68682F930EC6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$K$64</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$K$66</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="103">
   <si>
     <t>Item</t>
   </si>
@@ -233,9 +233,6 @@
     <t>Database build on plugin activation</t>
   </si>
   <si>
-    <t>Provide options on plugin deactivation</t>
-  </si>
-  <si>
     <t>Hide zoom link</t>
   </si>
   <si>
@@ -338,26 +335,27 @@
     <t>Replace Drop Down Menu to V2</t>
   </si>
   <si>
-    <t>Hold</t>
-  </si>
-  <si>
     <t>Nonces are handled automatically by Gutenberg and the Rest API for block editor.  There will be a need when frontend editing is enabled.</t>
+  </si>
+  <si>
+    <t>Deleting it broke the block.  Have not looked at code alternatives</t>
+  </si>
+  <si>
+    <t>Add Table Name field to table creation page</t>
+  </si>
+  <si>
+    <t>In Process</t>
+  </si>
+  <si>
+    <t>Provide options on plugin uninstall</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -397,12 +395,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -418,9 +415,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -736,63 +732,63 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9A95F50-2338-43A7-B2D8-210D78A54828}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:O66"/>
+  <dimension ref="A1:O67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="59.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" style="6" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" style="5" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="64.28515625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="59.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" style="4" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="64.28515625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="N1" s="9"/>
-      <c r="O1" s="10"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="8"/>
     </row>
     <row r="2" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -915,13 +911,13 @@
         <v>51</v>
       </c>
       <c r="B6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
         <v>81</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" t="s">
-        <v>82</v>
       </c>
       <c r="E6" t="s">
         <v>6</v>
@@ -940,182 +936,182 @@
       <c r="K6"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+      <c r="A7" s="4">
         <v>49</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C7" s="5" t="s">
+      <c r="B7" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="4">
+        <v>1</v>
+      </c>
+      <c r="H7" s="5">
+        <v>17</v>
+      </c>
+      <c r="I7" s="4">
+        <v>1</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>32</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>33</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="4">
+        <v>1</v>
+      </c>
+      <c r="I9" s="4">
+        <v>3</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>34</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="4">
+        <v>1</v>
+      </c>
+      <c r="I10" s="4">
+        <v>2</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>50</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E7" s="5" t="s">
+      <c r="C11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="5">
-        <v>1</v>
-      </c>
-      <c r="H7" s="6">
-        <v>17</v>
-      </c>
-      <c r="I7" s="5">
-        <v>1</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+      <c r="F11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="4">
+        <v>1</v>
+      </c>
+      <c r="H11" s="5">
         <v>32</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="G8" s="5">
-        <v>1</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
-        <v>33</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="5" t="s">
+      <c r="I11" s="4">
+        <v>3</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>35</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="5">
-        <v>1</v>
-      </c>
-      <c r="I9" s="5">
-        <v>3</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
-        <v>34</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="5">
-        <v>1</v>
-      </c>
-      <c r="I10" s="5">
+      <c r="E12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="4">
+        <v>1</v>
+      </c>
+      <c r="I12" s="4">
         <v>4</v>
       </c>
-      <c r="J10" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
-        <v>50</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G11" s="5">
-        <v>1</v>
-      </c>
-      <c r="H11" s="6">
-        <v>32</v>
-      </c>
-      <c r="I11" s="5">
-        <v>5</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
-        <v>35</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G12" s="5">
-        <v>1</v>
-      </c>
-      <c r="I12" s="5">
-        <v>6</v>
-      </c>
-      <c r="J12" s="5" t="s">
+      <c r="J12" s="4" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1124,7 +1120,7 @@
         <v>41</v>
       </c>
       <c r="B13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C13" t="s">
         <v>17</v>
@@ -1143,7 +1139,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13"/>
-      <c r="J13" s="2" t="s">
+      <c r="J13" t="s">
         <v>26</v>
       </c>
       <c r="K13"/>
@@ -1153,7 +1149,7 @@
         <v>42</v>
       </c>
       <c r="B14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C14" t="s">
         <v>17</v>
@@ -1172,95 +1168,95 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14"/>
-      <c r="J14" s="2" t="s">
+      <c r="J14" t="s">
         <v>26</v>
       </c>
       <c r="K14"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
+      <c r="A15" s="4">
         <v>46</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" s="4">
+        <v>1</v>
+      </c>
+      <c r="I15" s="4">
+        <v>5</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>47</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D16" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E15" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G15" s="5">
-        <v>1</v>
-      </c>
-      <c r="I15" s="5">
-        <v>9</v>
-      </c>
-      <c r="J15" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
-        <v>47</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" s="5" t="s">
+      <c r="E16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" s="4">
+        <v>1</v>
+      </c>
+      <c r="I16" s="4">
+        <v>6</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>58</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E16" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G16" s="5">
-        <v>1</v>
-      </c>
-      <c r="I16" s="5">
-        <v>10</v>
-      </c>
-      <c r="J16" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
-        <v>58</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G17" s="5">
-        <v>1</v>
-      </c>
-      <c r="I17" s="5">
-        <v>11</v>
-      </c>
-      <c r="J17" s="5" t="s">
+      <c r="E17" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" s="4">
+        <v>1</v>
+      </c>
+      <c r="I17" s="4">
+        <v>7</v>
+      </c>
+      <c r="J17" s="4" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1269,10 +1265,10 @@
         <v>59</v>
       </c>
       <c r="B18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D18" t="s">
         <v>56</v>
@@ -1288,7 +1284,7 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18"/>
-      <c r="J18" s="2" t="s">
+      <c r="J18" t="s">
         <v>26</v>
       </c>
       <c r="K18"/>
@@ -1298,7 +1294,7 @@
         <v>48</v>
       </c>
       <c r="B19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C19" t="s">
         <v>17</v>
@@ -1317,154 +1313,157 @@
       </c>
       <c r="H19" s="1"/>
       <c r="I19"/>
-      <c r="J19" s="2" t="s">
+      <c r="J19" t="s">
         <v>26</v>
       </c>
       <c r="K19"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="5">
+      <c r="A20" s="4">
         <v>62</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" s="4">
+        <v>1</v>
+      </c>
+      <c r="I20" s="4">
+        <v>8</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>63</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C21" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D21" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E20" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G20" s="5">
-        <v>1</v>
-      </c>
-      <c r="I20" s="5">
-        <v>14</v>
-      </c>
-      <c r="J20" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="5">
-        <v>63</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C21" s="5" t="s">
+      <c r="E21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" s="4">
+        <v>1</v>
+      </c>
+      <c r="I21" s="4">
+        <v>9</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>36</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" s="4">
+        <v>1</v>
+      </c>
+      <c r="I22" s="4">
+        <v>10</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>43</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D23" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E21" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G21" s="5">
-        <v>1</v>
-      </c>
-      <c r="I21" s="5">
-        <v>15</v>
-      </c>
-      <c r="J21" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="5">
-        <v>36</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E22" s="5" t="s">
+      <c r="E23" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F22" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G22" s="5">
-        <v>1</v>
-      </c>
-      <c r="I22" s="5">
-        <v>16</v>
-      </c>
-      <c r="J22" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="5">
-        <v>43</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D23" s="5" t="s">
+      <c r="F23" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23" s="4">
+        <v>1</v>
+      </c>
+      <c r="I23" s="4">
+        <v>11</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
         <v>56</v>
       </c>
-      <c r="E23" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G23" s="5">
-        <v>1</v>
-      </c>
-      <c r="I23" s="5">
-        <v>17</v>
-      </c>
-      <c r="J23" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="5">
+      <c r="B24" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D24" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G24" s="5">
-        <v>1</v>
-      </c>
-      <c r="I24" s="5">
-        <v>18</v>
-      </c>
-      <c r="J24" s="5" t="s">
-        <v>27</v>
+      <c r="E24" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" s="4">
+        <v>1</v>
+      </c>
+      <c r="I24" s="4">
+        <v>12</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -2154,466 +2153,491 @@
       <c r="K49"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="5">
+      <c r="A50" s="4">
         <v>57</v>
       </c>
-      <c r="B50" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="D50" s="5" t="s">
+      <c r="B50" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D50" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E50" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G50" s="5">
-        <v>1</v>
-      </c>
-      <c r="I50" s="5">
+      <c r="E50" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G50" s="4">
+        <v>1</v>
+      </c>
+      <c r="I50" s="4">
+        <v>13</v>
+      </c>
+      <c r="J50" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="4">
+        <v>60</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G51" s="4">
+        <v>1</v>
+      </c>
+      <c r="I51" s="4">
+        <v>14</v>
+      </c>
+      <c r="J51" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="4">
+        <v>38</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G52" s="4">
+        <v>1</v>
+      </c>
+      <c r="H52" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="I52" s="4">
+        <v>15</v>
+      </c>
+      <c r="J52" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K52" s="6"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="4">
+        <v>39</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G53" s="4">
+        <v>1</v>
+      </c>
+      <c r="I53" s="4">
+        <v>16</v>
+      </c>
+      <c r="J53" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="4">
+        <v>40</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G54" s="4">
+        <v>1</v>
+      </c>
+      <c r="I54" s="4">
+        <v>17</v>
+      </c>
+      <c r="J54" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="4">
+        <v>44</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G55" s="4">
+        <v>1</v>
+      </c>
+      <c r="I55" s="4">
+        <v>18</v>
+      </c>
+      <c r="J55" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="4">
+        <v>45</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G56" s="4">
+        <v>1</v>
+      </c>
+      <c r="I56" s="4">
         <v>19</v>
       </c>
-      <c r="J50" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="5">
-        <v>60</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="D51" s="5" t="s">
+      <c r="J56" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" s="4">
+        <v>26</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G57" s="4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J57" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" s="4">
+        <v>29</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G58" s="4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J58" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" s="4">
+        <v>31</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F59" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G59" s="4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J59" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" s="4">
+        <v>52</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F60" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G60" s="4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J60" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" s="4">
+        <v>53</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F61" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G61" s="4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J61" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" s="4">
+        <v>54</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F62" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G62" s="4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J62" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" s="4">
+        <v>55</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F63" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G63" s="4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J63" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64" s="4">
+        <v>61</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D64" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E51" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G51" s="5">
-        <v>1</v>
-      </c>
-      <c r="I51" s="5">
-        <v>20</v>
-      </c>
-      <c r="J51" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="5">
-        <v>38</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D52" s="5" t="s">
+      <c r="E64" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F64" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G64" s="4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J64" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65" s="4">
+        <v>64</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C65" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="E52" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G52" s="5">
-        <v>1</v>
-      </c>
-      <c r="H52" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="I52" s="5">
-        <v>21</v>
-      </c>
-      <c r="J52" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="K52" s="7"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="5">
-        <v>39</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="E53" s="5" t="s">
+      <c r="D65" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F65" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G65" s="4">
+        <v>1</v>
+      </c>
+      <c r="J65" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66" s="4">
+        <v>65</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F66" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F53" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G53" s="5">
-        <v>1</v>
-      </c>
-      <c r="I53" s="5">
-        <v>22</v>
-      </c>
-      <c r="J53" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="5">
-        <v>40</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="E54" s="5" t="s">
+      <c r="G66" s="4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J66" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67" s="4">
+        <v>66</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F67" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F54" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G54" s="5">
-        <v>1</v>
-      </c>
-      <c r="I54" s="5">
-        <v>23</v>
-      </c>
-      <c r="J54" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="5">
-        <v>44</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E55" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F55" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G55" s="5">
-        <v>1</v>
-      </c>
-      <c r="I55" s="5">
-        <v>24</v>
-      </c>
-      <c r="J55" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="5">
-        <v>45</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E56" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F56" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G56" s="5">
-        <v>1</v>
-      </c>
-      <c r="I56" s="5">
-        <v>25</v>
-      </c>
-      <c r="J56" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="5">
-        <v>26</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E57" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F57" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G57" s="5">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="J57" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="5">
-        <v>29</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E58" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F58" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G58" s="5">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="J58" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" s="5">
-        <v>31</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E59" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F59" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G59" s="5">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="J59" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60" s="5">
-        <v>52</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E60" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F60" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G60" s="5">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="J60" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A61" s="5">
-        <v>53</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E61" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F61" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G61" s="5">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="J61" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A62" s="5">
-        <v>54</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E62" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F62" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G62" s="5">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="J62" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A63" s="5">
-        <v>55</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E63" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F63" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G63" s="5">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="J63" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A64" s="5">
-        <v>61</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D64" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E64" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F64" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G64" s="5">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="J64" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A65" s="5">
-        <v>64</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C65" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="D65" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E65" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F65" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G65" s="5">
-        <v>1</v>
-      </c>
-      <c r="J65" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A66" s="5">
-        <v>65</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C66" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="D66" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E66" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F66" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G66" s="5">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="J66" s="5" t="s">
-        <v>27</v>
+      <c r="G67" s="4">
+        <v>1</v>
+      </c>
+      <c r="J67" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:K64" xr:uid="{C9A95F50-2338-43A7-B2D8-210D78A54828}">
+  <autoFilter ref="B1:K66" xr:uid="{C9A95F50-2338-43A7-B2D8-210D78A54828}">
     <filterColumn colId="8">
       <filters>
         <filter val="Open"/>
-        <filter val="Researching"/>
         <filter val="Testing"/>
       </filters>
     </filterColumn>

</xml_diff>

<commit_message>
Verify number of columns/rows are reasonable
</commit_message>
<xml_diff>
--- a/Development Docs/ToDo.xlsx
+++ b/Development Docs/ToDo.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greg\Local Sites\schaub-labs\app\public\wp-content\plugins\dynamic-tables\Development Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{720200F6-2116-47EE-A2A4-EFD9F0D7C7CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A40CDD8-DF5F-4F4E-B377-ED9CBF03F3AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{A3DBE3D2-0DAF-4481-8DC4-68682F930EC6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="17520" xr2:uid="{A3DBE3D2-0DAF-4481-8DC4-68682F930EC6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$K$66</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$K$67</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -735,7 +735,7 @@
   <dimension ref="A1:O67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1340,11 +1340,8 @@
       <c r="G20" s="4">
         <v>1</v>
       </c>
-      <c r="I20" s="4">
-        <v>8</v>
-      </c>
       <c r="J20" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -2243,7 +2240,7 @@
       </c>
       <c r="K52" s="6"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>39</v>
       </c>
@@ -2607,7 +2604,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
         <v>66</v>
       </c>
@@ -2634,9 +2631,10 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:K66" xr:uid="{C9A95F50-2338-43A7-B2D8-210D78A54828}">
+  <autoFilter ref="B1:K67" xr:uid="{C9A95F50-2338-43A7-B2D8-210D78A54828}">
     <filterColumn colId="8">
       <filters>
+        <filter val="In Process"/>
         <filter val="Open"/>
         <filter val="Testing"/>
       </filters>

</xml_diff>

<commit_message>
Verify nbr of cols/rows are reasonable
</commit_message>
<xml_diff>
--- a/Development Docs/ToDo.xlsx
+++ b/Development Docs/ToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greg\Local Sites\schaub-labs\app\public\wp-content\plugins\dynamic-tables\Development Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A40CDD8-DF5F-4F4E-B377-ED9CBF03F3AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D195218-4C4E-4CD1-B64B-E43A05E6B0D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="17520" xr2:uid="{A3DBE3D2-0DAF-4481-8DC4-68682F930EC6}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$K$67</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$K$68</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="105">
   <si>
     <t>Item</t>
   </si>
@@ -348,14 +348,28 @@
   </si>
   <si>
     <t>Provide options on plugin uninstall</t>
+  </si>
+  <si>
+    <t>Fix:  Freeze Header Row makes header row hidden</t>
+  </si>
+  <si>
+    <t>Last Number Used</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -395,7 +409,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -417,6 +431,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -732,10 +749,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9A95F50-2338-43A7-B2D8-210D78A54828}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:O67"/>
+  <dimension ref="A1:O89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -790,166 +807,163 @@
       <c r="N1" s="7"/>
       <c r="O1" s="8"/>
     </row>
-    <row r="2" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>49</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="4">
+        <v>1</v>
+      </c>
+      <c r="H2" s="5">
+        <v>17</v>
+      </c>
+      <c r="I2" s="4">
+        <v>1</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>47</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="4">
+        <v>1</v>
+      </c>
+      <c r="I3" s="4">
+        <v>2</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>33</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="E4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2" s="1"/>
-      <c r="I2"/>
-      <c r="J2" t="s">
-        <v>26</v>
-      </c>
-      <c r="K2"/>
-    </row>
-    <row r="3" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3" s="1"/>
-      <c r="I3"/>
-      <c r="J3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K3"/>
-    </row>
-    <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4" s="1"/>
-      <c r="I4"/>
-      <c r="J4" t="s">
-        <v>26</v>
-      </c>
-      <c r="K4"/>
+      <c r="G4" s="4">
+        <v>1</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>17</v>
-      </c>
-      <c r="B5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5" s="1"/>
-      <c r="I5"/>
-      <c r="J5" t="s">
-        <v>26</v>
-      </c>
-      <c r="K5"/>
-    </row>
-    <row r="6" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>51</v>
-      </c>
-      <c r="B6" t="s">
-        <v>80</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" t="s">
-        <v>81</v>
-      </c>
-      <c r="E6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6" s="1"/>
-      <c r="I6"/>
-      <c r="J6" t="s">
-        <v>26</v>
-      </c>
-      <c r="K6"/>
+      <c r="A5" s="4">
+        <v>64</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="4">
+        <v>1</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>60</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="4">
+        <v>1</v>
+      </c>
+      <c r="I6" s="4">
+        <v>3</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>75</v>
+        <v>17</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>56</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>7</v>
@@ -957,118 +971,119 @@
       <c r="G7" s="4">
         <v>1</v>
       </c>
-      <c r="H7" s="5">
+      <c r="I7" s="4">
+        <v>4</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>63</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="4">
-        <v>1</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
-        <v>32</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="D8" s="4" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="G8" s="4">
-        <v>1.1000000000000001</v>
+        <v>1</v>
+      </c>
+      <c r="I8" s="4">
+        <v>5</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="K8" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>32</v>
+        <v>103</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G9" s="4">
         <v>1</v>
       </c>
       <c r="I9" s="4">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>18</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G10" s="4">
         <v>1</v>
       </c>
+      <c r="H10" s="5" t="s">
+        <v>79</v>
+      </c>
       <c r="I10" s="4">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="K10" s="6"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>18</v>
+        <v>93</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>7</v>
@@ -1076,11 +1091,8 @@
       <c r="G11" s="4">
         <v>1</v>
       </c>
-      <c r="H11" s="5">
-        <v>32</v>
-      </c>
       <c r="I11" s="4">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="J11" s="4" t="s">
         <v>27</v>
@@ -1088,115 +1100,115 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="4">
+        <v>1</v>
+      </c>
+      <c r="I12" s="4">
+        <v>9</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
         <v>39</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G12" s="4">
-        <v>1</v>
-      </c>
-      <c r="I12" s="4">
-        <v>4</v>
-      </c>
-      <c r="J12" s="4" t="s">
+      <c r="B13" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="4">
+        <v>1</v>
+      </c>
+      <c r="I13" s="4">
+        <v>16</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>43</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" s="4">
+        <v>1</v>
+      </c>
+      <c r="I14" s="4">
+        <v>10</v>
+      </c>
+      <c r="J14" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>41</v>
-      </c>
-      <c r="B13" t="s">
-        <v>64</v>
-      </c>
-      <c r="C13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" t="s">
-        <v>56</v>
-      </c>
-      <c r="E13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F13" t="s">
-        <v>7</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="H13" s="1"/>
-      <c r="I13"/>
-      <c r="J13" t="s">
-        <v>26</v>
-      </c>
-      <c r="K13"/>
-    </row>
-    <row r="14" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>42</v>
-      </c>
-      <c r="B14" t="s">
-        <v>65</v>
-      </c>
-      <c r="C14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" t="s">
-        <v>56</v>
-      </c>
-      <c r="E14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-      <c r="H14" s="1"/>
-      <c r="I14"/>
-      <c r="J14" t="s">
-        <v>26</v>
-      </c>
-      <c r="K14"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>69</v>
+        <v>37</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G15" s="4">
         <v>1</v>
       </c>
       <c r="I15" s="4">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="J15" s="4" t="s">
         <v>27</v>
@@ -1204,28 +1216,28 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>70</v>
+        <v>39</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="G16" s="4">
         <v>1</v>
       </c>
       <c r="I16" s="4">
-        <v>6</v>
+        <v>99</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>27</v>
@@ -1233,19 +1245,19 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>56</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>7</v>
@@ -1254,221 +1266,224 @@
         <v>1</v>
       </c>
       <c r="I17" s="4">
-        <v>7</v>
+        <v>99</v>
       </c>
       <c r="J17" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A18">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>45</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" s="4">
+        <v>1</v>
+      </c>
+      <c r="I18" s="4">
+        <v>99</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>50</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" s="4">
+        <v>1</v>
+      </c>
+      <c r="H19" s="5">
+        <v>32</v>
+      </c>
+      <c r="I19" s="4">
+        <v>99</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" t="s">
+        <v>6</v>
+      </c>
+      <c r="F20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20"/>
+      <c r="I20"/>
+      <c r="J20" t="s">
+        <v>26</v>
+      </c>
+      <c r="K20"/>
+    </row>
+    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21"/>
+      <c r="I21"/>
+      <c r="J21" t="s">
+        <v>26</v>
+      </c>
+      <c r="K21"/>
+    </row>
+    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" t="s">
+        <v>57</v>
+      </c>
+      <c r="E22" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22"/>
+      <c r="I22"/>
+      <c r="J22" t="s">
+        <v>26</v>
+      </c>
+      <c r="K22"/>
+    </row>
+    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>4</v>
+      </c>
+      <c r="B23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" t="s">
+        <v>57</v>
+      </c>
+      <c r="E23" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23"/>
+      <c r="I23"/>
+      <c r="J23" t="s">
+        <v>26</v>
+      </c>
+      <c r="K23"/>
+    </row>
+    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
         <v>59</v>
       </c>
-      <c r="B18" t="s">
-        <v>89</v>
-      </c>
-      <c r="C18" t="s">
-        <v>75</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="C24" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" t="s">
         <v>56</v>
       </c>
-      <c r="E18" t="s">
-        <v>6</v>
-      </c>
-      <c r="F18" t="s">
-        <v>7</v>
-      </c>
-      <c r="G18">
-        <v>1</v>
-      </c>
-      <c r="H18" s="1"/>
-      <c r="I18"/>
-      <c r="J18" t="s">
-        <v>26</v>
-      </c>
-      <c r="K18"/>
-    </row>
-    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>48</v>
-      </c>
-      <c r="B19" t="s">
-        <v>71</v>
-      </c>
-      <c r="C19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" t="s">
-        <v>56</v>
-      </c>
-      <c r="E19" t="s">
-        <v>6</v>
-      </c>
-      <c r="F19" t="s">
-        <v>7</v>
-      </c>
-      <c r="G19">
-        <v>1</v>
-      </c>
-      <c r="H19" s="1"/>
-      <c r="I19"/>
-      <c r="J19" t="s">
-        <v>26</v>
-      </c>
-      <c r="K19"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
-        <v>62</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G20" s="4">
-        <v>1</v>
-      </c>
-      <c r="J20" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
-        <v>63</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G21" s="4">
-        <v>1</v>
-      </c>
-      <c r="I21" s="4">
-        <v>9</v>
-      </c>
-      <c r="J21" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
-        <v>36</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G22" s="4">
-        <v>1</v>
-      </c>
-      <c r="I22" s="4">
-        <v>10</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
-        <v>43</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G23" s="4">
-        <v>1</v>
-      </c>
-      <c r="I23" s="4">
-        <v>11</v>
-      </c>
-      <c r="J23" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
-        <v>56</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G24" s="4">
-        <v>1</v>
-      </c>
-      <c r="I24" s="4">
-        <v>12</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="K24" s="4" t="s">
-        <v>99</v>
-      </c>
+      <c r="E24" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24"/>
+      <c r="I24"/>
+      <c r="J24" t="s">
+        <v>26</v>
+      </c>
+      <c r="K24"/>
     </row>
     <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C25" t="s">
         <v>18</v>
@@ -1490,16 +1505,14 @@
       <c r="J25" t="s">
         <v>26</v>
       </c>
-      <c r="K25">
-        <v>19</v>
-      </c>
+      <c r="K25"/>
     </row>
     <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C26" t="s">
         <v>18</v>
@@ -1521,16 +1534,14 @@
       <c r="J26" t="s">
         <v>26</v>
       </c>
-      <c r="K26">
-        <v>20</v>
-      </c>
+      <c r="K26"/>
     </row>
     <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C27" t="s">
         <v>18</v>
@@ -1552,16 +1563,14 @@
       <c r="J27" t="s">
         <v>26</v>
       </c>
-      <c r="K27">
-        <v>21</v>
-      </c>
+      <c r="K27"/>
     </row>
     <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B28" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C28" t="s">
         <v>18</v>
@@ -1583,22 +1592,20 @@
       <c r="J28" t="s">
         <v>26</v>
       </c>
-      <c r="K28">
-        <v>22</v>
-      </c>
+      <c r="K28"/>
     </row>
     <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B29" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C29" t="s">
         <v>18</v>
       </c>
       <c r="D29" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E29" t="s">
         <v>6</v>
@@ -1614,25 +1621,23 @@
       <c r="J29" t="s">
         <v>26</v>
       </c>
-      <c r="K29">
-        <v>23</v>
-      </c>
+      <c r="K29"/>
     </row>
     <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B30" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="C30" t="s">
         <v>18</v>
       </c>
       <c r="D30" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="E30" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="F30" t="s">
         <v>7</v>
@@ -1645,25 +1650,23 @@
       <c r="J30" t="s">
         <v>26</v>
       </c>
-      <c r="K30">
-        <v>14</v>
-      </c>
+      <c r="K30"/>
     </row>
     <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B31" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="C31" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D31" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="E31" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="F31" t="s">
         <v>7</v>
@@ -1680,19 +1683,19 @@
     </row>
     <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B32" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D32" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="E32" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="F32" t="s">
         <v>7</v>
@@ -1707,64 +1710,70 @@
       </c>
       <c r="K32"/>
     </row>
-    <row r="33" spans="1:10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B33" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C33" t="s">
         <v>18</v>
       </c>
       <c r="D33" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="E33" t="s">
         <v>6</v>
       </c>
       <c r="F33" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G33">
         <v>1</v>
       </c>
+      <c r="H33" s="1"/>
+      <c r="I33"/>
       <c r="J33" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="K33"/>
+    </row>
+    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B34" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C34" t="s">
         <v>18</v>
       </c>
       <c r="D34" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="E34" t="s">
         <v>6</v>
       </c>
       <c r="F34" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G34">
         <v>1</v>
       </c>
+      <c r="H34" s="1"/>
+      <c r="I34"/>
       <c r="J34" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="K34"/>
+    </row>
+    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B35" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="C35" t="s">
         <v>18</v>
@@ -1773,50 +1782,56 @@
         <v>21</v>
       </c>
       <c r="E35" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="F35" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G35">
         <v>1</v>
       </c>
+      <c r="H35" s="1"/>
+      <c r="I35"/>
       <c r="J35" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="K35"/>
+    </row>
+    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B36" t="s">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="C36" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D36" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E36" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="F36" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G36">
         <v>1</v>
       </c>
+      <c r="H36" s="1"/>
+      <c r="I36"/>
       <c r="J36" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="K36"/>
+    </row>
+    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B37" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="C37" t="s">
         <v>17</v>
@@ -1825,76 +1840,85 @@
         <v>20</v>
       </c>
       <c r="E37" t="s">
+        <v>6</v>
+      </c>
+      <c r="F37" t="s">
+        <v>7</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+      <c r="H37"/>
+      <c r="I37"/>
+      <c r="J37" t="s">
+        <v>26</v>
+      </c>
+      <c r="K37"/>
+    </row>
+    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>19</v>
+      </c>
+      <c r="B38" t="s">
+        <v>38</v>
+      </c>
+      <c r="C38" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" t="s">
+        <v>7</v>
+      </c>
+      <c r="G38">
+        <v>1</v>
+      </c>
+      <c r="H38"/>
+      <c r="I38"/>
+      <c r="J38" t="s">
+        <v>26</v>
+      </c>
+      <c r="K38"/>
+    </row>
+    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>20</v>
+      </c>
+      <c r="B39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" t="s">
+        <v>17</v>
+      </c>
+      <c r="D39" t="s">
+        <v>20</v>
+      </c>
+      <c r="E39" t="s">
         <v>25</v>
       </c>
-      <c r="F37" t="s">
-        <v>7</v>
-      </c>
-      <c r="G37">
-        <v>1</v>
-      </c>
-      <c r="J37" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>18</v>
-      </c>
-      <c r="B38" t="s">
-        <v>28</v>
-      </c>
-      <c r="C38" t="s">
-        <v>17</v>
-      </c>
-      <c r="D38" t="s">
-        <v>20</v>
-      </c>
-      <c r="E38" t="s">
-        <v>6</v>
-      </c>
-      <c r="F38" t="s">
-        <v>7</v>
-      </c>
-      <c r="G38">
-        <v>1</v>
-      </c>
-      <c r="J38" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>19</v>
-      </c>
-      <c r="B39" t="s">
-        <v>38</v>
-      </c>
-      <c r="C39" t="s">
-        <v>18</v>
-      </c>
-      <c r="D39" t="s">
-        <v>9</v>
-      </c>
-      <c r="E39" t="s">
-        <v>11</v>
-      </c>
       <c r="F39" t="s">
         <v>7</v>
       </c>
       <c r="G39">
         <v>1</v>
       </c>
+      <c r="H39"/>
+      <c r="I39"/>
       <c r="J39" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="K39"/>
+    </row>
+    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B40" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="C40" t="s">
         <v>17</v>
@@ -1911,68 +1935,77 @@
       <c r="G40">
         <v>1</v>
       </c>
+      <c r="H40"/>
+      <c r="I40"/>
       <c r="J40" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="K40"/>
+    </row>
+    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41">
+        <v>22</v>
+      </c>
+      <c r="B41" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" t="s">
+        <v>18</v>
+      </c>
+      <c r="D41" t="s">
+        <v>4</v>
+      </c>
+      <c r="E41" t="s">
+        <v>6</v>
+      </c>
+      <c r="F41" t="s">
+        <v>7</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+      <c r="H41"/>
+      <c r="I41"/>
+      <c r="J41" t="s">
+        <v>26</v>
+      </c>
+      <c r="K41"/>
+    </row>
+    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>23</v>
+      </c>
+      <c r="B42" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" t="s">
         <v>21</v>
       </c>
-      <c r="B41" t="s">
-        <v>42</v>
-      </c>
-      <c r="C41" t="s">
-        <v>17</v>
-      </c>
-      <c r="D41" t="s">
-        <v>20</v>
-      </c>
-      <c r="E41" t="s">
+      <c r="E42" t="s">
         <v>25</v>
       </c>
-      <c r="F41" t="s">
-        <v>7</v>
-      </c>
-      <c r="G41">
-        <v>1</v>
-      </c>
-      <c r="J41" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>22</v>
-      </c>
-      <c r="B42" t="s">
-        <v>5</v>
-      </c>
-      <c r="C42" t="s">
-        <v>18</v>
-      </c>
-      <c r="D42" t="s">
-        <v>4</v>
-      </c>
-      <c r="E42" t="s">
-        <v>6</v>
-      </c>
       <c r="F42" t="s">
         <v>7</v>
       </c>
       <c r="G42">
         <v>1</v>
       </c>
+      <c r="H42"/>
+      <c r="I42"/>
       <c r="J42" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="K42"/>
+    </row>
+    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B43" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C43" t="s">
         <v>18</v>
@@ -1989,126 +2022,142 @@
       <c r="G43">
         <v>1</v>
       </c>
+      <c r="H43"/>
+      <c r="I43"/>
       <c r="J43" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="K43"/>
+    </row>
+    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B44" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C44" t="s">
         <v>18</v>
       </c>
       <c r="D44" t="s">
+        <v>9</v>
+      </c>
+      <c r="E44" t="s">
+        <v>11</v>
+      </c>
+      <c r="F44" t="s">
+        <v>7</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+      <c r="H44"/>
+      <c r="I44"/>
+      <c r="J44" t="s">
+        <v>26</v>
+      </c>
+      <c r="K44"/>
+    </row>
+    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>27</v>
+      </c>
+      <c r="B45" t="s">
+        <v>36</v>
+      </c>
+      <c r="C45" t="s">
+        <v>18</v>
+      </c>
+      <c r="D45" t="s">
         <v>21</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E45" t="s">
         <v>25</v>
       </c>
-      <c r="F44" t="s">
-        <v>7</v>
-      </c>
-      <c r="G44">
-        <v>1</v>
-      </c>
-      <c r="J44" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>25</v>
-      </c>
-      <c r="B45" t="s">
-        <v>8</v>
-      </c>
-      <c r="C45" t="s">
-        <v>18</v>
-      </c>
-      <c r="D45" t="s">
-        <v>9</v>
-      </c>
-      <c r="E45" t="s">
-        <v>11</v>
-      </c>
       <c r="F45" t="s">
         <v>7</v>
       </c>
       <c r="G45">
         <v>1</v>
       </c>
+      <c r="H45"/>
+      <c r="I45"/>
       <c r="J45" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="K45"/>
+    </row>
+    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B46" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="C46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D46" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="E46" t="s">
         <v>25</v>
       </c>
       <c r="F46" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="G46">
         <v>1</v>
       </c>
+      <c r="H46"/>
+      <c r="I46"/>
       <c r="J46" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="K46"/>
+    </row>
+    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B47" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="C47" t="s">
         <v>17</v>
       </c>
-      <c r="D47" t="s">
-        <v>56</v>
-      </c>
+      <c r="D47"/>
       <c r="E47" t="s">
         <v>25</v>
       </c>
       <c r="F47" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="G47">
         <v>1</v>
       </c>
+      <c r="H47"/>
+      <c r="I47"/>
       <c r="J47" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="K47"/>
+    </row>
+    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B48" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="C48" t="s">
         <v>17</v>
       </c>
+      <c r="D48" t="s">
+        <v>56</v>
+      </c>
       <c r="E48" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="F48" t="s">
         <v>11</v>
@@ -2116,16 +2165,19 @@
       <c r="G48">
         <v>1</v>
       </c>
+      <c r="H48"/>
+      <c r="I48"/>
       <c r="J48" t="s">
         <v>26</v>
       </c>
+      <c r="K48"/>
     </row>
     <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B49" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C49" t="s">
         <v>17</v>
@@ -2137,124 +2189,120 @@
         <v>6</v>
       </c>
       <c r="F49" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G49">
         <v>1</v>
       </c>
-      <c r="H49"/>
+      <c r="H49" s="1"/>
       <c r="I49"/>
       <c r="J49" t="s">
         <v>26</v>
       </c>
       <c r="K49"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="4">
-        <v>57</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D50" s="4" t="s">
+    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>42</v>
+      </c>
+      <c r="B50" t="s">
+        <v>65</v>
+      </c>
+      <c r="C50" t="s">
+        <v>17</v>
+      </c>
+      <c r="D50" t="s">
         <v>56</v>
       </c>
-      <c r="E50" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F50" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G50" s="4">
-        <v>1</v>
-      </c>
-      <c r="I50" s="4">
-        <v>13</v>
-      </c>
-      <c r="J50" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="4">
-        <v>60</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="D51" s="4" t="s">
+      <c r="E50" t="s">
+        <v>6</v>
+      </c>
+      <c r="F50" t="s">
+        <v>7</v>
+      </c>
+      <c r="G50">
+        <v>1</v>
+      </c>
+      <c r="H50" s="1"/>
+      <c r="I50"/>
+      <c r="J50" t="s">
+        <v>26</v>
+      </c>
+      <c r="K50"/>
+    </row>
+    <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>48</v>
+      </c>
+      <c r="B51" t="s">
+        <v>71</v>
+      </c>
+      <c r="C51" t="s">
+        <v>17</v>
+      </c>
+      <c r="D51" t="s">
         <v>56</v>
       </c>
-      <c r="E51" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F51" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G51" s="4">
-        <v>1</v>
-      </c>
-      <c r="I51" s="4">
-        <v>14</v>
-      </c>
-      <c r="J51" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="4">
-        <v>38</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E52" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F52" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G52" s="4">
-        <v>1</v>
-      </c>
-      <c r="H52" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="I52" s="4">
-        <v>15</v>
-      </c>
-      <c r="J52" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="K52" s="6"/>
+      <c r="E51" t="s">
+        <v>6</v>
+      </c>
+      <c r="F51" t="s">
+        <v>7</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
+      </c>
+      <c r="H51" s="1"/>
+      <c r="I51"/>
+      <c r="J51" t="s">
+        <v>26</v>
+      </c>
+      <c r="K51"/>
+    </row>
+    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>80</v>
+      </c>
+      <c r="C52" t="s">
+        <v>18</v>
+      </c>
+      <c r="D52" t="s">
+        <v>81</v>
+      </c>
+      <c r="E52" t="s">
+        <v>6</v>
+      </c>
+      <c r="F52" t="s">
+        <v>7</v>
+      </c>
+      <c r="G52">
+        <v>1</v>
+      </c>
+      <c r="H52" s="1"/>
+      <c r="I52"/>
+      <c r="J52" t="s">
+        <v>26</v>
+      </c>
+      <c r="K52"/>
     </row>
     <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>63</v>
+        <v>87</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>18</v>
+        <v>75</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F53" s="4" t="s">
         <v>7</v>
@@ -2262,57 +2310,54 @@
       <c r="G53" s="4">
         <v>1</v>
       </c>
-      <c r="I53" s="4">
-        <v>16</v>
-      </c>
       <c r="J53" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="4">
-        <v>40</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D54" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E54" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F54" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G54" s="4">
-        <v>1</v>
-      </c>
-      <c r="I54" s="4">
+    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>59</v>
+      </c>
+      <c r="B54" t="s">
+        <v>89</v>
+      </c>
+      <c r="C54" t="s">
+        <v>75</v>
+      </c>
+      <c r="D54" t="s">
+        <v>56</v>
+      </c>
+      <c r="E54" t="s">
+        <v>6</v>
+      </c>
+      <c r="F54" t="s">
+        <v>7</v>
+      </c>
+      <c r="G54">
+        <v>1</v>
+      </c>
+      <c r="H54" s="1"/>
+      <c r="I54"/>
+      <c r="J54" t="s">
+        <v>26</v>
+      </c>
+      <c r="K54"/>
+    </row>
+    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="4">
+        <v>62</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C55" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="J54" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="4">
-        <v>44</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>75</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>56</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="F55" s="4" t="s">
         <v>7</v>
@@ -2320,43 +2365,37 @@
       <c r="G55" s="4">
         <v>1</v>
       </c>
-      <c r="I55" s="4">
-        <v>18</v>
-      </c>
       <c r="J55" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>68</v>
+        <v>100</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>75</v>
+        <v>17</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>56</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G56" s="4">
         <v>1</v>
       </c>
-      <c r="I56" s="4">
-        <v>19</v>
-      </c>
       <c r="J56" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>26</v>
       </c>
@@ -2382,7 +2421,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
         <v>29</v>
       </c>
@@ -2408,7 +2447,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
         <v>31</v>
       </c>
@@ -2434,18 +2473,21 @@
         <v>27</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>82</v>
+        <v>29</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="D60" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="E60" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F60" s="4" t="s">
         <v>24</v>
@@ -2456,22 +2498,28 @@
       <c r="J60" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K60" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="D61" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="E61" s="4" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="G61" s="4">
         <v>1.1000000000000001</v>
@@ -2480,18 +2528,18 @@
         <v>27</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F62" s="4" t="s">
         <v>24</v>
@@ -2503,15 +2551,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E63" s="4" t="s">
         <v>25</v>
@@ -2526,24 +2574,21 @@
         <v>27</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D64" s="4" t="s">
-        <v>56</v>
-      </c>
       <c r="E64" s="4" t="s">
         <v>25</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="G64" s="4">
         <v>1.1000000000000001</v>
@@ -2552,47 +2597,44 @@
         <v>27</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D65" s="4" t="s">
-        <v>56</v>
+        <v>17</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="G65" s="4">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J65" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>93</v>
+        <v>17</v>
       </c>
       <c r="D66" s="4" t="s">
         <v>56</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="F66" s="4" t="s">
         <v>11</v>
@@ -2604,15 +2646,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>17</v>
+        <v>93</v>
       </c>
       <c r="D67" s="4" t="s">
         <v>56</v>
@@ -2624,14 +2666,60 @@
         <v>11</v>
       </c>
       <c r="G67" s="4">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A68" s="4">
+        <v>56</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F68" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G68" s="4">
+        <v>1</v>
+      </c>
+      <c r="I68" s="4">
+        <v>99</v>
+      </c>
+      <c r="J68" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K68" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="9">
+        <f>MAX(A2:A88)</f>
+        <v>67</v>
+      </c>
+      <c r="B89" s="9" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:K67" xr:uid="{C9A95F50-2338-43A7-B2D8-210D78A54828}">
+  <autoFilter ref="B1:K68" xr:uid="{C9A95F50-2338-43A7-B2D8-210D78A54828}">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="1"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="8">
       <filters>
         <filter val="In Process"/>
@@ -2643,10 +2731,10 @@
       <sortCondition ref="I2:I37"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:K69">
-    <sortCondition ref="G2:G69"/>
-    <sortCondition ref="I2:I69"/>
-    <sortCondition ref="A2:A69"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K68">
+    <sortCondition ref="G2:G68"/>
+    <sortCondition ref="I2:I68"/>
+    <sortCondition ref="A2:A68"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updates, fixes, and style enhancements
</commit_message>
<xml_diff>
--- a/Development Docs/ToDo.xlsx
+++ b/Development Docs/ToDo.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greg\Local Sites\schaub-labs\app\public\wp-content\plugins\dynamic-tables\Development Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D195218-4C4E-4CD1-B64B-E43A05E6B0D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA3E0803-E860-46AA-937B-DBFECBF176AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="17520" xr2:uid="{A3DBE3D2-0DAF-4481-8DC4-68682F930EC6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28020" windowHeight="14715" xr2:uid="{A3DBE3D2-0DAF-4481-8DC4-68682F930EC6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$K$68</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$K$69</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="136">
   <si>
     <t>Item</t>
   </si>
@@ -248,9 +249,6 @@
     <t>Remove console.log  statements</t>
   </si>
   <si>
-    <t>Fix styling on BorderBox controls</t>
-  </si>
-  <si>
     <t>Make # Rows/Columns read only and update style</t>
   </si>
   <si>
@@ -354,13 +352,109 @@
   </si>
   <si>
     <t>Last Number Used</t>
+  </si>
+  <si>
+    <t>Fix:  Styling on BorderBox controls</t>
+  </si>
+  <si>
+    <t>Editor</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>Editor Interface</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>attribute of EditorInterface call</t>
+  </si>
+  <si>
+    <t>entities-saved-states</t>
+  </si>
+  <si>
+    <t>Has function EntityTypeList</t>
+  </si>
+  <si>
+    <t>entity-type-list</t>
+  </si>
+  <si>
+    <t>Has function EntityTypeRecord</t>
+  </si>
+  <si>
+    <t>Produces list of items to save with a drop down header from entityLabel (i.e., Table from the Dynamic Tables entity config).</t>
+  </si>
+  <si>
+    <t>entity-record-item</t>
+  </si>
+  <si>
+    <t>Produces the list items to be saved</t>
+  </si>
+  <si>
+    <t>All from the entity type in the type list</t>
+  </si>
+  <si>
+    <t>Identifier is the title from "experimentalGetTemplateInfo" in the Editor Store (we show "untitled" on the save screen for Dynamic Tables)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - odd that it is tied to the template and not the entity</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - only retrieves dirty entity records where entity "kind" !== postType and "name" !== wp_template</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   + our name = table, kind = dynamic-tables/v1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - the "template" is the entity to be saved.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - I think an entity attribute of "title" would result in something more relevant than "Untitled"</t>
+  </si>
+  <si>
+    <t>Produces save/cancel buttons with prompt "Are you ready to save?"</t>
+  </si>
+  <si>
+    <t>save-publish-panels</t>
+  </si>
+  <si>
+    <t>Identifies dirty entities editor store that are NOT the post in the editor</t>
+  </si>
+  <si>
+    <t>Controls open/close of save panel and opens it on save when needed</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Passes the 4 attributes into the call (close, is, set callback, dirty for SavePublishPanels</t>
+  </si>
+  <si>
+    <t>Run customSavePanel || SavePublishPanels if not in preview</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - customSavePanel passed as prop of EditorInterface (calling function)</t>
+  </si>
+  <si>
+    <t>Tables are allowed to expand to fit the columns if Horizontal Scroll is not selected.  The overflow-x is set to "clip".  Setting overflow-x to "hidden" would retain the table width, but the columns right of the table boundry would be inaccessible if the rows are not allowed to grow.</t>
+  </si>
+  <si>
+    <t>Need to complete component "ConfigureRowHeight"</t>
+  </si>
+  <si>
+    <t>Limit block width to the with of all grid columns</t>
+  </si>
+  <si>
+    <t>Doesn't appear to be possible.  Opened Gutenberg issue (bug) #68771 on 1/19/2025</t>
+  </si>
+  <si>
+    <t>Doesn't appear to be possible.  Opened Gutenberg issue (bug) #68772 on 1/19/2025</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -371,6 +465,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -409,7 +511,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -434,6 +536,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -751,8 +854,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:O89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -772,7 +875,7 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -790,10 +893,10 @@
         <v>3</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>23</v>
@@ -812,10 +915,10 @@
         <v>49</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>56</v>
@@ -836,18 +939,18 @@
         <v>1</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>47</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>17</v>
+        <v>92</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>56</v>
@@ -865,44 +968,53 @@
         <v>2</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>33</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>32</v>
+        <v>104</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G4" s="4">
         <v>1</v>
       </c>
+      <c r="I4" s="4">
+        <v>3</v>
+      </c>
       <c r="J4" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>96</v>
+        <v>133</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>56</v>
@@ -916,8 +1028,11 @@
       <c r="G5" s="4">
         <v>1</v>
       </c>
+      <c r="I5" s="4">
+        <v>4</v>
+      </c>
       <c r="J5" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -925,16 +1040,16 @@
         <v>60</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>90</v>
+        <v>22</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>93</v>
+        <v>17</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>7</v>
@@ -943,10 +1058,13 @@
         <v>1</v>
       </c>
       <c r="I6" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>27</v>
+        <v>100</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -954,10 +1072,10 @@
         <v>46</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>69</v>
+        <v>102</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>56</v>
@@ -972,7 +1090,7 @@
         <v>1</v>
       </c>
       <c r="I7" s="4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J7" s="4" t="s">
         <v>27</v>
@@ -983,16 +1101,16 @@
         <v>63</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>95</v>
+        <v>62</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>7</v>
@@ -1000,22 +1118,26 @@
       <c r="G8" s="4">
         <v>1</v>
       </c>
+      <c r="H8" s="5" t="s">
+        <v>78</v>
+      </c>
       <c r="I8" s="4">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="K8" s="6"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>67</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>40</v>
+        <v>92</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>56</v>
@@ -1030,7 +1152,7 @@
         <v>1</v>
       </c>
       <c r="I9" s="4">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>27</v>
@@ -1041,16 +1163,16 @@
         <v>38</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>62</v>
+        <v>101</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>18</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>7</v>
@@ -1058,32 +1180,28 @@
       <c r="G10" s="4">
         <v>1</v>
       </c>
-      <c r="H10" s="5" t="s">
-        <v>79</v>
-      </c>
       <c r="I10" s="4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="K10" s="6"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>58</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>93</v>
+        <v>18</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>7</v>
@@ -1092,10 +1210,10 @@
         <v>1</v>
       </c>
       <c r="I11" s="4">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -1103,13 +1221,13 @@
         <v>40</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>102</v>
+        <v>66</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>11</v>
@@ -1121,39 +1239,39 @@
         <v>1</v>
       </c>
       <c r="I12" s="4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>39</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>74</v>
+        <v>31</v>
       </c>
       <c r="E13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="4" t="s">
-        <v>7</v>
-      </c>
       <c r="G13" s="4">
         <v>1</v>
       </c>
       <c r="I13" s="4">
-        <v>16</v>
+        <v>99</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -1161,25 +1279,25 @@
         <v>43</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="G14" s="4">
         <v>1</v>
       </c>
       <c r="I14" s="4">
-        <v>10</v>
+        <v>99</v>
       </c>
       <c r="J14" s="4" t="s">
         <v>27</v>
@@ -1190,19 +1308,19 @@
         <v>34</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G15" s="4">
         <v>1</v>
@@ -1219,19 +1337,19 @@
         <v>35</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="G16" s="4">
         <v>1</v>
@@ -1248,22 +1366,25 @@
         <v>44</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>75</v>
+        <v>18</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>7</v>
       </c>
       <c r="G17" s="4">
         <v>1</v>
+      </c>
+      <c r="H17" s="5">
+        <v>32</v>
       </c>
       <c r="I17" s="4">
         <v>99</v>
@@ -1272,21 +1393,21 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>45</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>75</v>
+        <v>17</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>56</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>7</v>
@@ -1294,19 +1415,16 @@
       <c r="G18" s="4">
         <v>1</v>
       </c>
-      <c r="I18" s="4">
-        <v>99</v>
-      </c>
       <c r="J18" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>50</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>76</v>
+        <v>32</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>18</v>
@@ -1315,88 +1433,79 @@
         <v>31</v>
       </c>
       <c r="E19" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="4" t="s">
-        <v>7</v>
-      </c>
       <c r="G19" s="4">
         <v>1</v>
       </c>
-      <c r="H19" s="5">
-        <v>32</v>
-      </c>
-      <c r="I19" s="4">
-        <v>99</v>
-      </c>
       <c r="J19" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1</v>
       </c>
-      <c r="B20" t="s">
-        <v>52</v>
-      </c>
-      <c r="C20" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20" t="s">
-        <v>57</v>
-      </c>
-      <c r="E20" t="s">
-        <v>6</v>
-      </c>
-      <c r="F20" t="s">
-        <v>7</v>
-      </c>
-      <c r="G20">
-        <v>1</v>
-      </c>
-      <c r="H20"/>
-      <c r="I20"/>
-      <c r="J20" t="s">
-        <v>26</v>
-      </c>
-      <c r="K20"/>
-    </row>
-    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" s="4">
+        <v>1</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2</v>
       </c>
-      <c r="B21" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21" t="s">
-        <v>57</v>
-      </c>
-      <c r="E21" t="s">
-        <v>6</v>
-      </c>
-      <c r="F21" t="s">
-        <v>7</v>
-      </c>
-      <c r="G21">
-        <v>1</v>
-      </c>
-      <c r="H21"/>
-      <c r="I21"/>
-      <c r="J21" t="s">
-        <v>26</v>
-      </c>
-      <c r="K21"/>
+      <c r="B21" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" s="4">
+        <v>1</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C22" t="s">
         <v>18</v>
@@ -1425,7 +1534,7 @@
         <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C23" t="s">
         <v>18</v>
@@ -1454,13 +1563,13 @@
         <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="C24" t="s">
         <v>18</v>
       </c>
       <c r="D24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E24" t="s">
         <v>6</v>
@@ -1483,7 +1592,7 @@
         <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C25" t="s">
         <v>18</v>
@@ -1512,13 +1621,13 @@
         <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="C26" t="s">
         <v>18</v>
       </c>
       <c r="D26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E26" t="s">
         <v>6</v>
@@ -1541,7 +1650,7 @@
         <v>8</v>
       </c>
       <c r="B27" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C27" t="s">
         <v>18</v>
@@ -1570,7 +1679,7 @@
         <v>9</v>
       </c>
       <c r="B28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C28" t="s">
         <v>18</v>
@@ -1599,7 +1708,7 @@
         <v>10</v>
       </c>
       <c r="B29" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C29" t="s">
         <v>18</v>
@@ -1628,16 +1737,16 @@
         <v>11</v>
       </c>
       <c r="B30" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="C30" t="s">
         <v>18</v>
       </c>
       <c r="D30" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="E30" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="F30" t="s">
         <v>7</v>
@@ -1657,16 +1766,16 @@
         <v>12</v>
       </c>
       <c r="B31" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="C31" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D31" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="E31" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="F31" t="s">
         <v>7</v>
@@ -1686,13 +1795,13 @@
         <v>13</v>
       </c>
       <c r="B32" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C32" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D32" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E32" t="s">
         <v>25</v>
@@ -1715,24 +1824,24 @@
         <v>14</v>
       </c>
       <c r="B33" t="s">
-        <v>53</v>
+        <v>13</v>
       </c>
       <c r="C33" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D33" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="E33" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="F33" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G33">
         <v>1</v>
       </c>
-      <c r="H33" s="1"/>
+      <c r="H33"/>
       <c r="I33"/>
       <c r="J33" t="s">
         <v>26</v>
@@ -1744,24 +1853,24 @@
         <v>15</v>
       </c>
       <c r="B34" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="C34" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D34" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E34" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="F34" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G34">
         <v>1</v>
       </c>
-      <c r="H34" s="1"/>
+      <c r="H34"/>
       <c r="I34"/>
       <c r="J34" t="s">
         <v>26</v>
@@ -1773,13 +1882,13 @@
         <v>16</v>
       </c>
       <c r="B35" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C35" t="s">
         <v>18</v>
       </c>
       <c r="D35" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="E35" t="s">
         <v>6</v>
@@ -1802,7 +1911,7 @@
         <v>17</v>
       </c>
       <c r="B36" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C36" t="s">
         <v>18</v>
@@ -1831,24 +1940,24 @@
         <v>18</v>
       </c>
       <c r="B37" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="C37" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D37" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E37" t="s">
         <v>6</v>
       </c>
       <c r="F37" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G37">
         <v>1</v>
       </c>
-      <c r="H37"/>
+      <c r="H37" s="1"/>
       <c r="I37"/>
       <c r="J37" t="s">
         <v>26</v>
@@ -1860,24 +1969,24 @@
         <v>19</v>
       </c>
       <c r="B38" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="C38" t="s">
         <v>18</v>
       </c>
       <c r="D38" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E38" t="s">
+        <v>6</v>
+      </c>
+      <c r="F38" t="s">
         <v>11</v>
       </c>
-      <c r="F38" t="s">
-        <v>7</v>
-      </c>
       <c r="G38">
         <v>1</v>
       </c>
-      <c r="H38"/>
+      <c r="H38" s="1"/>
       <c r="I38"/>
       <c r="J38" t="s">
         <v>26</v>
@@ -1889,7 +1998,7 @@
         <v>20</v>
       </c>
       <c r="B39" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="C39" t="s">
         <v>17</v>
@@ -1898,7 +2007,7 @@
         <v>20</v>
       </c>
       <c r="E39" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="F39" t="s">
         <v>7</v>
@@ -1918,16 +2027,16 @@
         <v>21</v>
       </c>
       <c r="B40" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C40" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D40" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E40" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F40" t="s">
         <v>7</v>
@@ -1947,16 +2056,16 @@
         <v>22</v>
       </c>
       <c r="B41" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C41" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D41" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="E41" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="F41" t="s">
         <v>7</v>
@@ -1976,13 +2085,13 @@
         <v>23</v>
       </c>
       <c r="B42" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="C42" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D42" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E42" t="s">
         <v>25</v>
@@ -2005,16 +2114,16 @@
         <v>24</v>
       </c>
       <c r="B43" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C43" t="s">
         <v>18</v>
       </c>
       <c r="D43" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="E43" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="F43" t="s">
         <v>7</v>
@@ -2034,16 +2143,16 @@
         <v>25</v>
       </c>
       <c r="B44" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C44" t="s">
         <v>18</v>
       </c>
       <c r="D44" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E44" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="F44" t="s">
         <v>7</v>
@@ -2063,7 +2172,7 @@
         <v>27</v>
       </c>
       <c r="B45" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="C45" t="s">
         <v>18</v>
@@ -2092,19 +2201,19 @@
         <v>28</v>
       </c>
       <c r="B46" t="s">
-        <v>60</v>
+        <v>8</v>
       </c>
       <c r="C46" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D46" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="E46" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F46" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="G46">
         <v>1</v>
@@ -2121,17 +2230,19 @@
         <v>30</v>
       </c>
       <c r="B47" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="C47" t="s">
-        <v>17</v>
-      </c>
-      <c r="D47"/>
+        <v>18</v>
+      </c>
+      <c r="D47" t="s">
+        <v>21</v>
+      </c>
       <c r="E47" t="s">
         <v>25</v>
       </c>
       <c r="F47" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G47">
         <v>1</v>
@@ -2148,7 +2259,7 @@
         <v>37</v>
       </c>
       <c r="B48" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C48" t="s">
         <v>17</v>
@@ -2157,10 +2268,10 @@
         <v>56</v>
       </c>
       <c r="E48" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="F48" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="G48">
         <v>1</v>
@@ -2177,24 +2288,22 @@
         <v>41</v>
       </c>
       <c r="B49" t="s">
-        <v>64</v>
+        <v>19</v>
       </c>
       <c r="C49" t="s">
         <v>17</v>
       </c>
-      <c r="D49" t="s">
-        <v>56</v>
-      </c>
+      <c r="D49"/>
       <c r="E49" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="F49" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G49">
         <v>1</v>
       </c>
-      <c r="H49" s="1"/>
+      <c r="H49"/>
       <c r="I49"/>
       <c r="J49" t="s">
         <v>26</v>
@@ -2206,7 +2315,7 @@
         <v>42</v>
       </c>
       <c r="B50" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C50" t="s">
         <v>17</v>
@@ -2218,12 +2327,12 @@
         <v>6</v>
       </c>
       <c r="F50" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G50">
         <v>1</v>
       </c>
-      <c r="H50" s="1"/>
+      <c r="H50"/>
       <c r="I50"/>
       <c r="J50" t="s">
         <v>26</v>
@@ -2235,7 +2344,7 @@
         <v>48</v>
       </c>
       <c r="B51" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C51" t="s">
         <v>17</v>
@@ -2264,13 +2373,13 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="C52" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D52" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="E52" t="s">
         <v>6</v>
@@ -2292,40 +2401,43 @@
       <c r="A53" s="4">
         <v>57</v>
       </c>
-      <c r="B53" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D53" s="4" t="s">
+      <c r="B53" t="s">
+        <v>70</v>
+      </c>
+      <c r="C53" t="s">
+        <v>17</v>
+      </c>
+      <c r="D53" t="s">
         <v>56</v>
       </c>
-      <c r="E53" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F53" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G53" s="4">
-        <v>1</v>
-      </c>
-      <c r="J53" s="4" t="s">
-        <v>26</v>
-      </c>
+      <c r="E53" t="s">
+        <v>6</v>
+      </c>
+      <c r="F53" t="s">
+        <v>7</v>
+      </c>
+      <c r="G53">
+        <v>1</v>
+      </c>
+      <c r="H53" s="1"/>
+      <c r="I53"/>
+      <c r="J53" t="s">
+        <v>26</v>
+      </c>
+      <c r="K53"/>
     </row>
     <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>59</v>
       </c>
       <c r="B54" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C54" t="s">
-        <v>75</v>
+        <v>18</v>
       </c>
       <c r="D54" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="E54" t="s">
         <v>6</v>
@@ -2348,10 +2460,10 @@
         <v>62</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>17</v>
+        <v>74</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>56</v>
@@ -2373,52 +2485,55 @@
       <c r="A56" s="4">
         <v>66</v>
       </c>
-      <c r="B56" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D56" s="4" t="s">
+      <c r="B56" t="s">
+        <v>88</v>
+      </c>
+      <c r="C56" t="s">
+        <v>74</v>
+      </c>
+      <c r="D56" t="s">
         <v>56</v>
       </c>
-      <c r="E56" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F56" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G56" s="4">
-        <v>1</v>
-      </c>
-      <c r="J56" s="4" t="s">
-        <v>26</v>
-      </c>
+      <c r="E56" t="s">
+        <v>6</v>
+      </c>
+      <c r="F56" t="s">
+        <v>7</v>
+      </c>
+      <c r="G56">
+        <v>1</v>
+      </c>
+      <c r="H56" s="1"/>
+      <c r="I56"/>
+      <c r="J56" t="s">
+        <v>26</v>
+      </c>
+      <c r="K56"/>
     </row>
     <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>26</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>35</v>
+        <v>93</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="G57" s="4">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -2426,59 +2541,65 @@
         <v>29</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>30</v>
+        <v>99</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="E58" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="G58" s="4">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="J58" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
         <v>31</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>22</v>
+        <v>85</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>17</v>
+        <v>74</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="G59" s="4">
-        <v>1.1000000000000001</v>
+        <v>1</v>
+      </c>
+      <c r="I59" s="4">
+        <v>99</v>
       </c>
       <c r="J59" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="K59" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
         <v>32</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>18</v>
@@ -2487,7 +2608,7 @@
         <v>21</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="F60" s="4" t="s">
         <v>24</v>
@@ -2498,16 +2619,13 @@
       <c r="J60" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="K60" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
         <v>36</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>18</v>
@@ -2516,10 +2634,10 @@
         <v>31</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="G61" s="4">
         <v>1.1000000000000001</v>
@@ -2528,18 +2646,21 @@
         <v>27</v>
       </c>
     </row>
-    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>52</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>82</v>
+        <v>29</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="D62" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="E62" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F62" s="4" t="s">
         <v>24</v>
@@ -2550,22 +2671,28 @@
       <c r="J62" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="K62" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <v>53</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="D63" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="E63" s="4" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="G63" s="4">
         <v>1.1000000000000001</v>
@@ -2574,18 +2701,18 @@
         <v>27</v>
       </c>
     </row>
-    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <v>54</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F64" s="4" t="s">
         <v>24</v>
@@ -2597,15 +2724,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>55</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E65" s="4" t="s">
         <v>25</v>
@@ -2620,24 +2747,21 @@
         <v>27</v>
       </c>
     </row>
-    <row r="66" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
         <v>61</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D66" s="4" t="s">
-        <v>56</v>
-      </c>
       <c r="E66" s="4" t="s">
         <v>25</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="G66" s="4">
         <v>1.1000000000000001</v>
@@ -2646,24 +2770,21 @@
         <v>27</v>
       </c>
     </row>
-    <row r="67" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
         <v>65</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="D67" s="4" t="s">
-        <v>56</v>
+        <v>17</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="G67" s="4">
         <v>1.1000000000000001</v>
@@ -2672,63 +2793,78 @@
         <v>27</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
         <v>56</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>75</v>
+        <v>17</v>
       </c>
       <c r="D68" s="4" t="s">
         <v>56</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G68" s="4">
-        <v>1</v>
-      </c>
-      <c r="I68" s="4">
-        <v>99</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J68" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="K68" s="4" t="s">
-        <v>99</v>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69" s="4">
+        <v>68</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F69" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G69" s="4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J69" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="9">
         <f>MAX(A2:A88)</f>
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B89" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:K68" xr:uid="{C9A95F50-2338-43A7-B2D8-210D78A54828}">
-    <filterColumn colId="5">
-      <filters>
-        <filter val="1"/>
-      </filters>
-    </filterColumn>
+  <autoFilter ref="B1:K69" xr:uid="{C9A95F50-2338-43A7-B2D8-210D78A54828}">
     <filterColumn colId="8">
-      <filters>
+      <filters blank="1">
         <filter val="In Process"/>
         <filter val="Open"/>
         <filter val="Testing"/>
       </filters>
     </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:K37">
-      <sortCondition ref="I2:I37"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:K69">
+      <sortCondition ref="I1:I69"/>
     </sortState>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K68">
@@ -2739,4 +2875,170 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9D206C0-E6E2-47CC-9389-62C309532CCD}">
+  <dimension ref="B9:T43"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9" t="s">
+        <v>106</v>
+      </c>
+      <c r="D9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="T16" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>105</v>
+      </c>
+      <c r="C19" t="s">
+        <v>106</v>
+      </c>
+      <c r="D19" t="s">
+        <v>107</v>
+      </c>
+      <c r="E19" t="s">
+        <v>108</v>
+      </c>
+      <c r="G19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G20" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G21" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>105</v>
+      </c>
+      <c r="C24" t="s">
+        <v>106</v>
+      </c>
+      <c r="D24" t="s">
+        <v>125</v>
+      </c>
+      <c r="E24" t="s">
+        <v>108</v>
+      </c>
+      <c r="G24" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G25" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>105</v>
+      </c>
+      <c r="C29" t="s">
+        <v>106</v>
+      </c>
+      <c r="D29" t="s">
+        <v>110</v>
+      </c>
+      <c r="E29" t="s">
+        <v>108</v>
+      </c>
+      <c r="G29" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G30" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="33" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>112</v>
+      </c>
+      <c r="G33" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="34" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="G34" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="36" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>115</v>
+      </c>
+      <c r="G36" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="37" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="G37" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="38" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="G38" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="39" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="G39" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="40" spans="5:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G40" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="41" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="G41" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="42" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="G42" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="43" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="G43" t="s">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add table title for save confirmation
</commit_message>
<xml_diff>
--- a/Development Docs/ToDo.xlsx
+++ b/Development Docs/ToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greg\Local Sites\schaub-labs\app\public\wp-content\plugins\dynamic-tables\Development Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA3E0803-E860-46AA-937B-DBFECBF176AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56FAEDBC-705E-4EA4-AF26-49BEF66597F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28020" windowHeight="14715" xr2:uid="{A3DBE3D2-0DAF-4481-8DC4-68682F930EC6}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$K$69</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$K$71</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="138">
   <si>
     <t>Item</t>
   </si>
@@ -444,10 +444,16 @@
     <t>Limit block width to the with of all grid columns</t>
   </si>
   <si>
-    <t>Doesn't appear to be possible.  Opened Gutenberg issue (bug) #68771 on 1/19/2025</t>
-  </si>
-  <si>
-    <t>Doesn't appear to be possible.  Opened Gutenberg issue (bug) #68772 on 1/19/2025</t>
+    <t>Remove the option to save specific table blocks after the save/publish post button has been pushed  Refer to issue 47</t>
+  </si>
+  <si>
+    <t>Opened Gutenberg issue (bug) #68771 on 1/19/2025.  Was able to update the entity so that the entity tile is displayed, but it still requires an additional confirmation and the ability to uncheck the entiy (Block) for save.  This is bad user experience and even has the potential to have data appear to save, but not actually persist.  There is a request to address the underlying "double confirmation" in issue #38714.  Created issue 70 to track the Gutenberg teams response/update to this issue.</t>
+  </si>
+  <si>
+    <t>Opened Gutenberg issue (bug) #68772 on 1/19/2025.  Team provided a workaround for the CSS.  This is a temporary fix.  Track progress of final solution through item 71.</t>
+  </si>
+  <si>
+    <t>Track resolution to Gutenberg issue  #68772 and remove workaround when final solution is in place.  Reference item 33.</t>
   </si>
 </sst>
 </file>
@@ -854,9 +860,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:O89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -942,7 +946,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>47</v>
       </c>
@@ -964,17 +968,14 @@
       <c r="G3" s="4">
         <v>1</v>
       </c>
-      <c r="I3" s="4">
-        <v>2</v>
-      </c>
       <c r="J3" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>33</v>
       </c>
@@ -996,14 +997,11 @@
       <c r="G4" s="4">
         <v>1</v>
       </c>
-      <c r="I4" s="4">
-        <v>3</v>
-      </c>
       <c r="J4" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -1029,7 +1027,7 @@
         <v>1</v>
       </c>
       <c r="I5" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>27</v>
@@ -1058,7 +1056,7 @@
         <v>1</v>
       </c>
       <c r="I6" s="4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J6" s="4" t="s">
         <v>100</v>
@@ -1090,7 +1088,7 @@
         <v>1</v>
       </c>
       <c r="I7" s="4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J7" s="4" t="s">
         <v>27</v>
@@ -1122,7 +1120,7 @@
         <v>78</v>
       </c>
       <c r="I8" s="4">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>27</v>
@@ -1152,7 +1150,7 @@
         <v>1</v>
       </c>
       <c r="I9" s="4">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>27</v>
@@ -1181,7 +1179,7 @@
         <v>1</v>
       </c>
       <c r="I10" s="4">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>100</v>
@@ -2845,19 +2843,71 @@
         <v>27</v>
       </c>
     </row>
+    <row r="70" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A70" s="4">
+        <v>70</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F70" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G70" s="4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J70" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A71" s="4">
+        <v>71</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F71" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G71" s="4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J71" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="9">
         <f>MAX(A2:A88)</f>
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B89" s="9" t="s">
         <v>103</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:K69" xr:uid="{C9A95F50-2338-43A7-B2D8-210D78A54828}">
+  <autoFilter ref="B1:K71" xr:uid="{C9A95F50-2338-43A7-B2D8-210D78A54828}">
     <filterColumn colId="8">
-      <filters blank="1">
+      <filters>
         <filter val="In Process"/>
         <filter val="Open"/>
         <filter val="Testing"/>

</xml_diff>

<commit_message>
Allow row height configuration
</commit_message>
<xml_diff>
--- a/Development Docs/ToDo.xlsx
+++ b/Development Docs/ToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greg\Local Sites\schaub-labs\app\public\wp-content\plugins\dynamic-tables\Development Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56FAEDBC-705E-4EA4-AF26-49BEF66597F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A934DE2-89A3-4576-BA88-AE765F62A5A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28020" windowHeight="14715" xr2:uid="{A3DBE3D2-0DAF-4481-8DC4-68682F930EC6}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="137">
   <si>
     <t>Item</t>
   </si>
@@ -330,9 +330,6 @@
     <t>Validate  nbr Rows/Cols are reasonable</t>
   </si>
   <si>
-    <t>Replace Drop Down Menu to V2</t>
-  </si>
-  <si>
     <t>Nonces are handled automatically by Gutenberg and the Rest API for block editor.  There will be a need when frontend editing is enabled.</t>
   </si>
   <si>
@@ -438,9 +435,6 @@
     <t>Tables are allowed to expand to fit the columns if Horizontal Scroll is not selected.  The overflow-x is set to "clip".  Setting overflow-x to "hidden" would retain the table width, but the columns right of the table boundry would be inaccessible if the rows are not allowed to grow.</t>
   </si>
   <si>
-    <t>Need to complete component "ConfigureRowHeight"</t>
-  </si>
-  <si>
     <t>Limit block width to the with of all grid columns</t>
   </si>
   <si>
@@ -454,6 +448,9 @@
   </si>
   <si>
     <t>Track resolution to Gutenberg issue  #68772 and remove workaround when final solution is in place.  Reference item 33.</t>
+  </si>
+  <si>
+    <t>Replace "DropdownMenu" to "Menu" (currently experimental/locked)</t>
   </si>
 </sst>
 </file>
@@ -860,7 +857,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:O89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -972,7 +971,7 @@
         <v>26</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -980,7 +979,7 @@
         <v>33</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>17</v>
@@ -1001,15 +1000,15 @@
         <v>26</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>69</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>92</v>
@@ -1026,14 +1025,11 @@
       <c r="G5" s="4">
         <v>1</v>
       </c>
-      <c r="I5" s="4">
-        <v>2</v>
-      </c>
       <c r="J5" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>60</v>
       </c>
@@ -1055,22 +1051,16 @@
       <c r="G6" s="4">
         <v>1</v>
       </c>
-      <c r="I6" s="4">
-        <v>3</v>
-      </c>
       <c r="J6" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>46</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>40</v>
@@ -1087,11 +1077,8 @@
       <c r="G7" s="4">
         <v>1</v>
       </c>
-      <c r="I7" s="4">
-        <v>4</v>
-      </c>
       <c r="J7" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -1120,7 +1107,7 @@
         <v>78</v>
       </c>
       <c r="I8" s="4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>27</v>
@@ -1150,7 +1137,7 @@
         <v>1</v>
       </c>
       <c r="I9" s="4">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>27</v>
@@ -1161,7 +1148,7 @@
         <v>38</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>18</v>
@@ -1179,10 +1166,10 @@
         <v>1</v>
       </c>
       <c r="I10" s="4">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
@@ -1381,9 +1368,6 @@
       <c r="G17" s="4">
         <v>1</v>
       </c>
-      <c r="H17" s="5">
-        <v>32</v>
-      </c>
       <c r="I17" s="4">
         <v>99</v>
       </c>
@@ -1495,7 +1479,7 @@
         <v>26</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -2539,7 +2523,7 @@
         <v>29</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>17</v>
@@ -2589,7 +2573,7 @@
         <v>27</v>
       </c>
       <c r="K59" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
@@ -2670,7 +2654,7 @@
         <v>27</v>
       </c>
       <c r="K62" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
@@ -2817,12 +2801,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
         <v>68</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>96</v>
+        <v>136</v>
       </c>
       <c r="C69" s="4" t="s">
         <v>92</v>
@@ -2848,7 +2832,7 @@
         <v>70</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C70" s="4" t="s">
         <v>92</v>
@@ -2874,7 +2858,7 @@
         <v>71</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C71" s="4" t="s">
         <v>92</v>
@@ -2901,7 +2885,7 @@
         <v>71</v>
       </c>
       <c r="B89" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -2944,148 +2928,148 @@
   <sheetData>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C9" t="s">
         <v>105</v>
       </c>
-      <c r="C9" t="s">
-        <v>106</v>
-      </c>
       <c r="D9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
       <c r="T16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
+        <v>104</v>
+      </c>
+      <c r="C19" t="s">
         <v>105</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>106</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>107</v>
       </c>
-      <c r="E19" t="s">
-        <v>108</v>
-      </c>
       <c r="G19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
+        <v>104</v>
+      </c>
+      <c r="C24" t="s">
         <v>105</v>
       </c>
-      <c r="C24" t="s">
-        <v>106</v>
-      </c>
       <c r="D24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G25" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
+        <v>104</v>
+      </c>
+      <c r="C29" t="s">
         <v>105</v>
       </c>
-      <c r="C29" t="s">
-        <v>106</v>
-      </c>
       <c r="D29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E29" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G29" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G30" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="33" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E33" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G33" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34" spans="5:7" x14ac:dyDescent="0.25">
       <c r="G34" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="36" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E36" t="s">
+        <v>114</v>
+      </c>
+      <c r="G36" t="s">
         <v>115</v>
-      </c>
-      <c r="G36" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="37" spans="5:7" x14ac:dyDescent="0.25">
       <c r="G37" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="38" spans="5:7" x14ac:dyDescent="0.25">
       <c r="G38" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="39" spans="5:7" x14ac:dyDescent="0.25">
       <c r="G39" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="40" spans="5:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G40" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="41" spans="5:7" x14ac:dyDescent="0.25">
       <c r="G41" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="42" spans="5:7" x14ac:dyDescent="0.25">
       <c r="G42" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="43" spans="5:7" x14ac:dyDescent="0.25">
       <c r="G43" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Create main admin pg, begin refactor for WP cd std
</commit_message>
<xml_diff>
--- a/Development Docs/ToDo.xlsx
+++ b/Development Docs/ToDo.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greg\Local Sites\schaub-labs\app\public\wp-content\plugins\dynamic-tables\Development Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A934DE2-89A3-4576-BA88-AE765F62A5A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C91BBC32-5278-4CFA-8B2A-444D182D6524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28020" windowHeight="14715" xr2:uid="{A3DBE3D2-0DAF-4481-8DC4-68682F930EC6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{A3DBE3D2-0DAF-4481-8DC4-68682F930EC6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$K$71</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$K$72</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="143">
   <si>
     <t>Item</t>
   </si>
@@ -294,9 +294,6 @@
     <t>Create admin page to maintain tables</t>
   </si>
   <si>
-    <t>Create table from CSV file</t>
-  </si>
-  <si>
     <t>Determine if useEffect for # col/row is still needed</t>
   </si>
   <si>
@@ -451,6 +448,27 @@
   </si>
   <si>
     <t>Replace "DropdownMenu" to "Menu" (currently experimental/locked)</t>
+  </si>
+  <si>
+    <t>Create complementary block to link a post containing details from a row in a table back to the post with the table</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Roadmap</t>
+  </si>
+  <si>
+    <t>Import table from CSV file</t>
+  </si>
+  <si>
+    <t>Export all tables</t>
+  </si>
+  <si>
+    <t>Export table (data only)</t>
+  </si>
+  <si>
+    <t>Export table (full object)</t>
   </si>
 </sst>
 </file>
@@ -858,7 +876,7 @@
   <dimension ref="A1:O89"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="K70" sqref="K70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -942,7 +960,7 @@
         <v>1</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="120" hidden="1" x14ac:dyDescent="0.25">
@@ -950,10 +968,10 @@
         <v>47</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>56</v>
@@ -971,7 +989,7 @@
         <v>26</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -979,7 +997,7 @@
         <v>33</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>17</v>
@@ -1000,7 +1018,7 @@
         <v>26</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
@@ -1008,10 +1026,10 @@
         <v>69</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>56</v>
@@ -1060,7 +1078,7 @@
         <v>46</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>40</v>
@@ -1119,10 +1137,10 @@
         <v>67</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>56</v>
@@ -1148,7 +1166,7 @@
         <v>38</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>18</v>
@@ -1169,7 +1187,7 @@
         <v>4</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
@@ -1432,7 +1450,7 @@
         <v>1</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>74</v>
@@ -1458,7 +1476,7 @@
         <v>2</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>17</v>
@@ -1479,7 +1497,7 @@
         <v>26</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -2442,7 +2460,7 @@
         <v>62</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>74</v>
@@ -2468,7 +2486,7 @@
         <v>66</v>
       </c>
       <c r="B56" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C56" t="s">
         <v>74</v>
@@ -2497,7 +2515,7 @@
         <v>26</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>17</v>
@@ -2523,7 +2541,7 @@
         <v>29</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>17</v>
@@ -2549,7 +2567,7 @@
         <v>31</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>74</v>
@@ -2573,7 +2591,7 @@
         <v>27</v>
       </c>
       <c r="K59" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
@@ -2654,7 +2672,7 @@
         <v>27</v>
       </c>
       <c r="K62" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
@@ -2757,7 +2775,7 @@
         <v>65</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>84</v>
+        <v>139</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>17</v>
@@ -2780,7 +2798,7 @@
         <v>56</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C68" s="4" t="s">
         <v>17</v>
@@ -2806,10 +2824,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D69" s="4" t="s">
         <v>56</v>
@@ -2832,10 +2850,10 @@
         <v>70</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D70" s="4" t="s">
         <v>56</v>
@@ -2858,10 +2876,10 @@
         <v>71</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D71" s="4" t="s">
         <v>56</v>
@@ -2877,23 +2895,128 @@
       </c>
       <c r="J71" s="4" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" s="4">
+        <v>72</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F72" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G72" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="J72" s="4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A73" s="4">
+        <v>73</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F73" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G73" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="J73" s="4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A74" s="4">
+        <v>74</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F74" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G74" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="J74" s="4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A75" s="4">
+        <v>75</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E75" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F75" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G75" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="J75" s="4" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="9">
         <f>MAX(A2:A88)</f>
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B89" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:K71" xr:uid="{C9A95F50-2338-43A7-B2D8-210D78A54828}">
+  <autoFilter ref="B1:K72" xr:uid="{C9A95F50-2338-43A7-B2D8-210D78A54828}">
     <filterColumn colId="8">
       <filters>
         <filter val="In Process"/>
         <filter val="Open"/>
+        <filter val="Roadmap"/>
         <filter val="Testing"/>
       </filters>
     </filterColumn>
@@ -2928,148 +3051,148 @@
   <sheetData>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" t="s">
         <v>104</v>
       </c>
-      <c r="C9" t="s">
-        <v>105</v>
-      </c>
       <c r="D9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
       <c r="T16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
+        <v>103</v>
+      </c>
+      <c r="C19" t="s">
         <v>104</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>105</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>106</v>
       </c>
-      <c r="E19" t="s">
-        <v>107</v>
-      </c>
       <c r="G19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G20" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G21" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
+        <v>103</v>
+      </c>
+      <c r="C24" t="s">
         <v>104</v>
       </c>
-      <c r="C24" t="s">
-        <v>105</v>
-      </c>
       <c r="D24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
+        <v>103</v>
+      </c>
+      <c r="C29" t="s">
         <v>104</v>
       </c>
-      <c r="C29" t="s">
-        <v>105</v>
-      </c>
       <c r="D29" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E29" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G29" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G30" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="33" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E33" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G33" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="34" spans="5:7" x14ac:dyDescent="0.25">
       <c r="G34" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="36" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E36" t="s">
+        <v>113</v>
+      </c>
+      <c r="G36" t="s">
         <v>114</v>
-      </c>
-      <c r="G36" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="37" spans="5:7" x14ac:dyDescent="0.25">
       <c r="G37" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="5:7" x14ac:dyDescent="0.25">
       <c r="G38" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="39" spans="5:7" x14ac:dyDescent="0.25">
       <c r="G39" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="40" spans="5:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G40" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="41" spans="5:7" x14ac:dyDescent="0.25">
       <c r="G41" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="42" spans="5:7" x14ac:dyDescent="0.25">
       <c r="G42" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="43" spans="5:7" x14ac:dyDescent="0.25">
       <c r="G43" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor render.php and code clean-up
</commit_message>
<xml_diff>
--- a/Development Docs/ToDo.xlsx
+++ b/Development Docs/ToDo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greg\Local Sites\schaub-labs\app\public\wp-content\plugins\dynamic-tables\Development Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C91BBC32-5278-4CFA-8B2A-444D182D6524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D81A189C-327C-46E9-8316-9B9F397B40C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{A3DBE3D2-0DAF-4481-8DC4-68682F930EC6}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$K$72</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$K$75</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="141">
   <si>
     <t>Item</t>
   </si>
@@ -276,9 +276,6 @@
     <t>Prereq</t>
   </si>
   <si>
-    <t>14, 49</t>
-  </si>
-  <si>
     <t>Populate PostId in table</t>
   </si>
   <si>
@@ -334,9 +331,6 @@
   </si>
   <si>
     <t>Add Table Name field to table creation page</t>
-  </si>
-  <si>
-    <t>In Process</t>
   </si>
   <si>
     <t>Provide options on plugin uninstall</t>
@@ -875,8 +869,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:O89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K70" sqref="K70"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -960,7 +954,7 @@
         <v>1</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="120" hidden="1" x14ac:dyDescent="0.25">
@@ -968,10 +962,10 @@
         <v>47</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>56</v>
@@ -989,7 +983,7 @@
         <v>26</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -997,7 +991,7 @@
         <v>33</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>17</v>
@@ -1018,7 +1012,7 @@
         <v>26</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
@@ -1026,10 +1020,10 @@
         <v>69</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>56</v>
@@ -1078,7 +1072,7 @@
         <v>46</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>40</v>
@@ -1099,7 +1093,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>63</v>
       </c>
@@ -1121,14 +1115,8 @@
       <c r="G8" s="4">
         <v>1</v>
       </c>
-      <c r="H8" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="I8" s="4">
-        <v>2</v>
-      </c>
       <c r="J8" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K8" s="6"/>
     </row>
@@ -1137,10 +1125,10 @@
         <v>67</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>56</v>
@@ -1155,18 +1143,18 @@
         <v>1</v>
       </c>
       <c r="I9" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>38</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>18</v>
@@ -1183,11 +1171,8 @@
       <c r="G10" s="4">
         <v>1</v>
       </c>
-      <c r="I10" s="4">
-        <v>4</v>
-      </c>
       <c r="J10" s="4" t="s">
-        <v>98</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
@@ -1450,7 +1435,7 @@
         <v>1</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>74</v>
@@ -1476,7 +1461,7 @@
         <v>2</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>17</v>
@@ -1497,7 +1482,7 @@
         <v>26</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -2431,13 +2416,13 @@
         <v>59</v>
       </c>
       <c r="B54" t="s">
+        <v>78</v>
+      </c>
+      <c r="C54" t="s">
+        <v>18</v>
+      </c>
+      <c r="D54" t="s">
         <v>79</v>
-      </c>
-      <c r="C54" t="s">
-        <v>18</v>
-      </c>
-      <c r="D54" t="s">
-        <v>80</v>
       </c>
       <c r="E54" t="s">
         <v>6</v>
@@ -2460,7 +2445,7 @@
         <v>62</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>74</v>
@@ -2486,7 +2471,7 @@
         <v>66</v>
       </c>
       <c r="B56" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C56" t="s">
         <v>74</v>
@@ -2515,7 +2500,7 @@
         <v>26</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>17</v>
@@ -2541,7 +2526,7 @@
         <v>29</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>17</v>
@@ -2567,7 +2552,7 @@
         <v>31</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>74</v>
@@ -2591,7 +2576,7 @@
         <v>27</v>
       </c>
       <c r="K59" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
@@ -2672,7 +2657,7 @@
         <v>27</v>
       </c>
       <c r="K62" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
@@ -2706,7 +2691,7 @@
         <v>54</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>18</v>
@@ -2729,7 +2714,7 @@
         <v>55</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>18</v>
@@ -2752,7 +2737,7 @@
         <v>61</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>17</v>
@@ -2775,7 +2760,7 @@
         <v>65</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>17</v>
@@ -2798,7 +2783,7 @@
         <v>56</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C68" s="4" t="s">
         <v>17</v>
@@ -2824,10 +2809,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D69" s="4" t="s">
         <v>56</v>
@@ -2850,10 +2835,10 @@
         <v>70</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D70" s="4" t="s">
         <v>56</v>
@@ -2876,10 +2861,10 @@
         <v>71</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D71" s="4" t="s">
         <v>56</v>
@@ -2902,13 +2887,13 @@
         <v>72</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C72" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E72" s="4" t="s">
         <v>25</v>
@@ -2917,10 +2902,10 @@
         <v>24</v>
       </c>
       <c r="G72" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J72" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
@@ -2928,13 +2913,13 @@
         <v>73</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C73" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E73" s="4" t="s">
         <v>25</v>
@@ -2943,10 +2928,10 @@
         <v>24</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J73" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
@@ -2954,13 +2939,13 @@
         <v>74</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C74" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E74" s="4" t="s">
         <v>25</v>
@@ -2969,10 +2954,10 @@
         <v>24</v>
       </c>
       <c r="G74" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J74" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
@@ -2980,13 +2965,13 @@
         <v>75</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C75" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E75" s="4" t="s">
         <v>25</v>
@@ -2995,10 +2980,10 @@
         <v>24</v>
       </c>
       <c r="G75" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J75" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
@@ -3007,14 +2992,13 @@
         <v>75</v>
       </c>
       <c r="B89" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:K72" xr:uid="{C9A95F50-2338-43A7-B2D8-210D78A54828}">
+  <autoFilter ref="B1:K75" xr:uid="{C9A95F50-2338-43A7-B2D8-210D78A54828}">
     <filterColumn colId="8">
       <filters>
-        <filter val="In Process"/>
         <filter val="Open"/>
         <filter val="Roadmap"/>
         <filter val="Testing"/>
@@ -3051,148 +3035,148 @@
   <sheetData>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D9" t="s">
+        <v>101</v>
+      </c>
+      <c r="E9" t="s">
         <v>104</v>
-      </c>
-      <c r="D9" t="s">
-        <v>103</v>
-      </c>
-      <c r="E9" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
       <c r="T16" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
+        <v>101</v>
+      </c>
+      <c r="C19" t="s">
+        <v>102</v>
+      </c>
+      <c r="D19" t="s">
         <v>103</v>
       </c>
-      <c r="C19" t="s">
+      <c r="E19" t="s">
         <v>104</v>
       </c>
-      <c r="D19" t="s">
-        <v>105</v>
-      </c>
-      <c r="E19" t="s">
-        <v>106</v>
-      </c>
       <c r="G19" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G20" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G21" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C24" t="s">
+        <v>102</v>
+      </c>
+      <c r="D24" t="s">
+        <v>121</v>
+      </c>
+      <c r="E24" t="s">
         <v>104</v>
       </c>
-      <c r="D24" t="s">
+      <c r="G24" t="s">
         <v>123</v>
-      </c>
-      <c r="E24" t="s">
-        <v>106</v>
-      </c>
-      <c r="G24" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G25" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C29" t="s">
+        <v>102</v>
+      </c>
+      <c r="D29" t="s">
+        <v>106</v>
+      </c>
+      <c r="E29" t="s">
         <v>104</v>
       </c>
-      <c r="D29" t="s">
-        <v>108</v>
-      </c>
-      <c r="E29" t="s">
-        <v>106</v>
-      </c>
       <c r="G29" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G30" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="33" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E33" t="s">
+        <v>108</v>
+      </c>
+      <c r="G33" t="s">
         <v>110</v>
-      </c>
-      <c r="G33" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="34" spans="5:7" x14ac:dyDescent="0.25">
       <c r="G34" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="36" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E36" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G36" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="37" spans="5:7" x14ac:dyDescent="0.25">
       <c r="G37" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="38" spans="5:7" x14ac:dyDescent="0.25">
       <c r="G38" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="39" spans="5:7" x14ac:dyDescent="0.25">
       <c r="G39" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="40" spans="5:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G40" s="10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="41" spans="5:7" x14ac:dyDescent="0.25">
       <c r="G41" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="42" spans="5:7" x14ac:dyDescent="0.25">
       <c r="G42" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="43" spans="5:7" x14ac:dyDescent="0.25">
       <c r="G43" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix deleted rows/cols not removed from DB
</commit_message>
<xml_diff>
--- a/Development Docs/ToDo.xlsx
+++ b/Development Docs/ToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greg\Local Sites\schaub-labs\app\public\wp-content\plugins\dynamic-tables\Development Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D81A189C-327C-46E9-8316-9B9F397B40C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F32D7AAA-608A-4381-BC97-A5E0057FA117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{A3DBE3D2-0DAF-4481-8DC4-68682F930EC6}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$K$75</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$K$77</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="147">
   <si>
     <t>Item</t>
   </si>
@@ -463,6 +463,24 @@
   </si>
   <si>
     <t>Export table (full object)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Performance is fine when testing on an full WP environment</t>
+  </si>
+  <si>
+    <t>Deleting columns and/or rows is not working</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>Enable update permissions for Rest API</t>
+  </si>
+  <si>
+    <t>Security</t>
   </si>
 </sst>
 </file>
@@ -870,7 +888,7 @@
   <dimension ref="A1:O89"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1120,7 +1138,7 @@
       </c>
       <c r="K8" s="6"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>67</v>
       </c>
@@ -1142,11 +1160,8 @@
       <c r="G9" s="4">
         <v>1</v>
       </c>
-      <c r="I9" s="4">
-        <v>2</v>
-      </c>
       <c r="J9" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
@@ -1204,7 +1219,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>40</v>
       </c>
@@ -1226,51 +1241,45 @@
       <c r="G12" s="4">
         <v>1</v>
       </c>
-      <c r="I12" s="4">
-        <v>10</v>
-      </c>
       <c r="J12" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>37</v>
+        <v>143</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>31</v>
+        <v>144</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G13" s="4">
         <v>1</v>
       </c>
-      <c r="I13" s="4">
-        <v>99</v>
-      </c>
       <c r="J13" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
-        <v>43</v>
+        <v>76</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>39</v>
+        <v>145</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>40</v>
+        <v>146</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>31</v>
@@ -1279,13 +1288,13 @@
         <v>6</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="G14" s="4">
         <v>1</v>
       </c>
       <c r="I14" s="4">
-        <v>99</v>
+        <v>2</v>
       </c>
       <c r="J14" s="4" t="s">
         <v>27</v>
@@ -1293,10 +1302,10 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>74</v>
@@ -1305,7 +1314,7 @@
         <v>56</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>7</v>
@@ -1319,13 +1328,16 @@
       <c r="J15" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="K15" s="4" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>74</v>
@@ -1349,7 +1361,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>44</v>
       </c>
@@ -1371,11 +1383,11 @@
       <c r="G17" s="4">
         <v>1</v>
       </c>
-      <c r="I17" s="4">
-        <v>99</v>
-      </c>
       <c r="J17" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -2549,10 +2561,10 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>74</v>
@@ -2561,7 +2573,7 @@
         <v>56</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="F59" s="4" t="s">
         <v>7</v>
@@ -2575,31 +2587,31 @@
       <c r="J59" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="K59" s="4" t="s">
-        <v>95</v>
-      </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>18</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="G60" s="4">
-        <v>1.1000000000000001</v>
+        <v>1</v>
+      </c>
+      <c r="I60" s="4">
+        <v>99</v>
       </c>
       <c r="J60" s="4" t="s">
         <v>27</v>
@@ -2607,13 +2619,13 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="D61" s="4" t="s">
         <v>31</v>
@@ -2625,18 +2637,21 @@
         <v>24</v>
       </c>
       <c r="G61" s="4">
-        <v>1.1000000000000001</v>
+        <v>1</v>
+      </c>
+      <c r="I61" s="4">
+        <v>99</v>
       </c>
       <c r="J61" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>18</v>
@@ -2645,7 +2660,7 @@
         <v>21</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="F62" s="4" t="s">
         <v>24</v>
@@ -2656,16 +2671,13 @@
       <c r="J62" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="K62" s="4" t="s">
-        <v>94</v>
-      </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>18</v>
@@ -2674,10 +2686,10 @@
         <v>31</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="G63" s="4">
         <v>1.1000000000000001</v>
@@ -2686,18 +2698,21 @@
         <v>27</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>80</v>
+        <v>29</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="D64" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="E64" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F64" s="4" t="s">
         <v>24</v>
@@ -2708,22 +2723,28 @@
       <c r="J64" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="K64" s="4" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>81</v>
+        <v>41</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="D65" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="E65" s="4" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="G65" s="4">
         <v>1.1000000000000001</v>
@@ -2734,16 +2755,16 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F66" s="4" t="s">
         <v>24</v>
@@ -2757,13 +2778,13 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>137</v>
+        <v>81</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E67" s="4" t="s">
         <v>25</v>
@@ -2804,24 +2825,21 @@
         <v>27</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>133</v>
+        <v>82</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="D69" s="4" t="s">
-        <v>56</v>
+        <v>17</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="G69" s="4">
         <v>1.1000000000000001</v>
@@ -2830,24 +2848,21 @@
         <v>27</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="D70" s="4" t="s">
-        <v>56</v>
+        <v>17</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="G70" s="4">
         <v>1.1000000000000001</v>
@@ -2858,10 +2873,10 @@
     </row>
     <row r="71" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C71" s="4" t="s">
         <v>90</v>
@@ -2873,7 +2888,7 @@
         <v>6</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="G71" s="4">
         <v>1.1000000000000001</v>
@@ -2884,62 +2899,62 @@
     </row>
     <row r="72" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>17</v>
+        <v>141</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>135</v>
+        <v>56</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G72" s="4" t="s">
-        <v>136</v>
+        <v>7</v>
+      </c>
+      <c r="G72" s="4">
+        <v>1.1000000000000001</v>
       </c>
       <c r="J72" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="4">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>17</v>
+        <v>90</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>135</v>
+        <v>56</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="F73" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G73" s="4" t="s">
-        <v>136</v>
+      <c r="G73" s="4">
+        <v>1.1000000000000001</v>
       </c>
       <c r="J73" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C74" s="4" t="s">
         <v>17</v>
@@ -2962,10 +2977,10 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="4">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C75" s="4" t="s">
         <v>17</v>
@@ -2983,20 +2998,72 @@
         <v>136</v>
       </c>
       <c r="J75" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="4">
+        <v>74</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E76" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F76" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G76" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="J76" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="4">
+        <v>75</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F77" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G77" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="J77" s="4" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="9">
         <f>MAX(A2:A88)</f>
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B89" s="9" t="s">
         <v>99</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:K75" xr:uid="{C9A95F50-2338-43A7-B2D8-210D78A54828}">
+  <autoFilter ref="B1:K77" xr:uid="{C9A95F50-2338-43A7-B2D8-210D78A54828}">
     <filterColumn colId="8">
       <filters>
         <filter val="Open"/>
@@ -3008,10 +3075,10 @@
       <sortCondition ref="I1:I69"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K68">
-    <sortCondition ref="G2:G68"/>
-    <sortCondition ref="I2:I68"/>
-    <sortCondition ref="A2:A68"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K77">
+    <sortCondition ref="G2:G77"/>
+    <sortCondition ref="I2:I77"/>
+    <sortCondition ref="A2:A77"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Misc javascript linting updates
</commit_message>
<xml_diff>
--- a/Development Docs/ToDo.xlsx
+++ b/Development Docs/ToDo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greg\Local Sites\schaub-labs\app\public\wp-content\plugins\dynamic-tables\Development Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F32D7AAA-608A-4381-BC97-A5E0057FA117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA899961-F62A-4EF6-96F4-133D85ACD194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{A3DBE3D2-0DAF-4481-8DC4-68682F930EC6}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="153">
   <si>
     <t>Item</t>
   </si>
@@ -243,9 +243,6 @@
     <t>Refactor render.php for structural changes</t>
   </si>
   <si>
-    <t>Remove document code</t>
-  </si>
-  <si>
     <t>Remove console.log  statements</t>
   </si>
   <si>
@@ -481,6 +478,27 @@
   </si>
   <si>
     <t>Security</t>
+  </si>
+  <si>
+    <t>Clean and document code</t>
+  </si>
+  <si>
+    <t>In Process</t>
+  </si>
+  <si>
+    <t>Add support to dynamically load table data (e.g., posts, csv)</t>
+  </si>
+  <si>
+    <t>Create Data Types on Columns</t>
+  </si>
+  <si>
+    <t>Create frontend interactivity to sort, filter, etc. table data</t>
+  </si>
+  <si>
+    <t>Add subscription capability</t>
+  </si>
+  <si>
+    <t>78, 80</t>
   </si>
 </sst>
 </file>
@@ -885,10 +903,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9A95F50-2338-43A7-B2D8-210D78A54828}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:O89"/>
+  <dimension ref="A1:O87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -908,7 +926,7 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -926,10 +944,10 @@
         <v>3</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>23</v>
@@ -948,10 +966,10 @@
         <v>49</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>56</v>
@@ -972,7 +990,7 @@
         <v>1</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="120" hidden="1" x14ac:dyDescent="0.25">
@@ -980,10 +998,10 @@
         <v>47</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>56</v>
@@ -1001,7 +1019,7 @@
         <v>26</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -1009,7 +1027,7 @@
         <v>33</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>17</v>
@@ -1030,7 +1048,7 @@
         <v>26</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
@@ -1038,10 +1056,10 @@
         <v>69</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>56</v>
@@ -1090,7 +1108,7 @@
         <v>46</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>40</v>
@@ -1122,7 +1140,7 @@
         <v>18</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>25</v>
@@ -1143,10 +1161,10 @@
         <v>67</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>56</v>
@@ -1169,13 +1187,13 @@
         <v>38</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>18</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>11</v>
@@ -1201,7 +1219,7 @@
         <v>18</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>11</v>
@@ -1250,13 +1268,13 @@
         <v>76</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>40</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>6</v>
@@ -1276,10 +1294,10 @@
         <v>76</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>145</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>146</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>31</v>
@@ -1305,16 +1323,16 @@
         <v>31</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>83</v>
+        <v>146</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>56</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>7</v>
@@ -1323,13 +1341,10 @@
         <v>1</v>
       </c>
       <c r="I15" s="4">
-        <v>99</v>
+        <v>3</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="K15" s="4" t="s">
-        <v>95</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -1340,7 +1355,7 @@
         <v>67</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>56</v>
@@ -1355,7 +1370,7 @@
         <v>1</v>
       </c>
       <c r="I16" s="4">
-        <v>99</v>
+        <v>4</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>27</v>
@@ -1366,7 +1381,7 @@
         <v>44</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>18</v>
@@ -1387,7 +1402,7 @@
         <v>26</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -1395,7 +1410,7 @@
         <v>45</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>17</v>
@@ -1447,10 +1462,10 @@
         <v>1</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>56</v>
@@ -1473,7 +1488,7 @@
         <v>2</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>17</v>
@@ -1494,7 +1509,7 @@
         <v>26</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -2399,7 +2414,7 @@
         <v>57</v>
       </c>
       <c r="B53" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C53" t="s">
         <v>17</v>
@@ -2428,13 +2443,13 @@
         <v>59</v>
       </c>
       <c r="B54" t="s">
+        <v>77</v>
+      </c>
+      <c r="C54" t="s">
+        <v>18</v>
+      </c>
+      <c r="D54" t="s">
         <v>78</v>
-      </c>
-      <c r="C54" t="s">
-        <v>18</v>
-      </c>
-      <c r="D54" t="s">
-        <v>79</v>
       </c>
       <c r="E54" t="s">
         <v>6</v>
@@ -2457,10 +2472,10 @@
         <v>62</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>56</v>
@@ -2483,10 +2498,10 @@
         <v>66</v>
       </c>
       <c r="B56" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C56" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D56" t="s">
         <v>56</v>
@@ -2512,7 +2527,7 @@
         <v>26</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>17</v>
@@ -2538,7 +2553,7 @@
         <v>29</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>17</v>
@@ -2564,16 +2579,16 @@
         <v>35</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>56</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="F59" s="4" t="s">
         <v>7</v>
@@ -2586,6 +2601,9 @@
       </c>
       <c r="J59" s="4" t="s">
         <v>27</v>
+      </c>
+      <c r="K59" s="4" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
@@ -2724,7 +2742,7 @@
         <v>27</v>
       </c>
       <c r="K64" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
@@ -2755,7 +2773,7 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B66" s="4" t="s">
         <v>80</v>
@@ -2764,7 +2782,7 @@
         <v>18</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="F66" s="4" t="s">
         <v>24</v>
@@ -2776,18 +2794,21 @@
         <v>27</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>81</v>
+        <v>132</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>18</v>
+        <v>89</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="F67" s="4" t="s">
         <v>24</v>
@@ -2799,24 +2820,24 @@
         <v>27</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>89</v>
+        <v>128</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="D68" s="4" t="s">
         <v>56</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="G68" s="4">
         <v>1.1000000000000001</v>
@@ -2825,18 +2846,21 @@
         <v>27</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>82</v>
+        <v>131</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>17</v>
+        <v>89</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="F69" s="4" t="s">
         <v>24</v>
@@ -2850,10 +2874,10 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>137</v>
+        <v>81</v>
       </c>
       <c r="C70" s="4" t="s">
         <v>17</v>
@@ -2861,205 +2885,327 @@
       <c r="E70" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F70" s="4" t="s">
+      <c r="G70" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="I70" s="5">
+        <v>1</v>
+      </c>
+      <c r="J70" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A71" s="4">
+        <v>74</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G71" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="I71" s="5">
+        <v>2</v>
+      </c>
+      <c r="J71" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A72" s="4">
+        <v>54</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F72" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G70" s="4">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="J70" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="4">
-        <v>68</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="D71" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E71" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F71" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G71" s="4">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="J71" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A72" s="4">
-        <v>70</v>
-      </c>
-      <c r="B72" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="D72" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E72" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F72" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G72" s="4">
-        <v>1.1000000000000001</v>
+      <c r="G72" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="H72" s="5">
+        <v>61</v>
+      </c>
+      <c r="I72" s="4">
+        <v>3</v>
       </c>
       <c r="J72" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="4">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>90</v>
+        <v>17</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>56</v>
+        <v>134</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F73" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G73" s="4">
-        <v>1.1000000000000001</v>
+        <v>25</v>
+      </c>
+      <c r="G73" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="I73" s="5">
+        <v>4</v>
       </c>
       <c r="J73" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>134</v>
+        <v>149</v>
       </c>
       <c r="C74" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E74" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F74" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="G74" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
+      </c>
+      <c r="I74" s="5">
+        <v>5</v>
       </c>
       <c r="J74" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="4">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>139</v>
+        <v>151</v>
       </c>
       <c r="C75" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E75" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F75" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="G75" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
+      </c>
+      <c r="I75" s="5">
+        <v>6</v>
       </c>
       <c r="J75" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="4">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="C76" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E76" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F76" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="G76" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
+      </c>
+      <c r="H76" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="I76" s="5">
+        <v>7</v>
       </c>
       <c r="J76" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="4">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>138</v>
+        <v>88</v>
       </c>
       <c r="C77" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>135</v>
+        <v>56</v>
       </c>
       <c r="E77" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F77" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="G77" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="I77" s="5">
+        <v>8</v>
+      </c>
+      <c r="J77" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="4">
+        <v>79</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E78" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G78" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="I78" s="5">
+        <v>9</v>
+      </c>
+      <c r="J78" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="4">
+        <v>65</v>
+      </c>
+      <c r="B79" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="J77" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="9">
-        <f>MAX(A2:A88)</f>
-        <v>76</v>
-      </c>
-      <c r="B89" s="9" t="s">
-        <v>99</v>
+      <c r="C79" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G79" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="I79" s="5">
+        <v>10</v>
+      </c>
+      <c r="J79" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="4">
+        <v>73</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G80" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="I80" s="5">
+        <v>11</v>
+      </c>
+      <c r="J80" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A81" s="4">
+        <v>72</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G81" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="I81" s="5">
+        <v>12</v>
+      </c>
+      <c r="J81" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I82" s="5"/>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I83" s="5"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I84" s="5"/>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I85" s="5"/>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I86" s="5"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="9">
+        <f>MAX(A1:A81)</f>
+        <v>80</v>
+      </c>
+      <c r="B87" s="9" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -3071,14 +3217,14 @@
         <filter val="Testing"/>
       </filters>
     </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:K69">
-      <sortCondition ref="I1:I69"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:K77">
+      <sortCondition ref="I1:I77"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K77">
-    <sortCondition ref="G2:G77"/>
-    <sortCondition ref="I2:I77"/>
-    <sortCondition ref="A2:A77"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K81">
+    <sortCondition ref="G2:G81"/>
+    <sortCondition ref="I2:I81"/>
+    <sortCondition ref="A2:A81"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3102,148 +3248,148 @@
   <sheetData>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" t="s">
         <v>101</v>
       </c>
-      <c r="C9" t="s">
-        <v>102</v>
-      </c>
       <c r="D9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
       <c r="T16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
+        <v>100</v>
+      </c>
+      <c r="C19" t="s">
         <v>101</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>102</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>103</v>
       </c>
-      <c r="E19" t="s">
-        <v>104</v>
-      </c>
       <c r="G19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G21" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
+        <v>100</v>
+      </c>
+      <c r="C24" t="s">
         <v>101</v>
       </c>
-      <c r="C24" t="s">
-        <v>102</v>
-      </c>
       <c r="D24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G25" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
+        <v>100</v>
+      </c>
+      <c r="C29" t="s">
         <v>101</v>
       </c>
-      <c r="C29" t="s">
-        <v>102</v>
-      </c>
       <c r="D29" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E29" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G29" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="33" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E33" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G33" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="34" spans="5:7" x14ac:dyDescent="0.25">
       <c r="G34" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="36" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E36" t="s">
+        <v>110</v>
+      </c>
+      <c r="G36" t="s">
         <v>111</v>
-      </c>
-      <c r="G36" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="37" spans="5:7" x14ac:dyDescent="0.25">
       <c r="G37" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="38" spans="5:7" x14ac:dyDescent="0.25">
       <c r="G38" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="39" spans="5:7" x14ac:dyDescent="0.25">
       <c r="G39" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="40" spans="5:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G40" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="41" spans="5:7" x14ac:dyDescent="0.25">
       <c r="G41" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="42" spans="5:7" x14ac:dyDescent="0.25">
       <c r="G42" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="43" spans="5:7" x14ac:dyDescent="0.25">
       <c r="G43" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix height for table rows without content
</commit_message>
<xml_diff>
--- a/Development Docs/ToDo.xlsx
+++ b/Development Docs/ToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greg\Local Sites\schaub-labs\app\public\wp-content\plugins\dynamic-tables\Development Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA899961-F62A-4EF6-96F4-133D85ACD194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37B31B14-9ECA-4035-94D8-2E835E354E0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{A3DBE3D2-0DAF-4481-8DC4-68682F930EC6}"/>
   </bookViews>
@@ -489,9 +489,6 @@
     <t>Add support to dynamically load table data (e.g., posts, csv)</t>
   </si>
   <si>
-    <t>Create Data Types on Columns</t>
-  </si>
-  <si>
     <t>Create frontend interactivity to sort, filter, etc. table data</t>
   </si>
   <si>
@@ -499,6 +496,9 @@
   </si>
   <si>
     <t>78, 80</t>
+  </si>
+  <si>
+    <t>Create Data Types on Columns (e.g., text, image, link/button, number, etc.)</t>
   </si>
 </sst>
 </file>
@@ -906,7 +906,7 @@
   <dimension ref="A1:O87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2976,12 +2976,12 @@
         <v>135</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
         <v>78</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="C74" s="4" t="s">
         <v>17</v>
@@ -3007,7 +3007,7 @@
         <v>80</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C75" s="4" t="s">
         <v>17</v>
@@ -3048,7 +3048,7 @@
         <v>135</v>
       </c>
       <c r="H76" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I76" s="5">
         <v>7</v>
@@ -3088,7 +3088,7 @@
         <v>79</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C78" s="4" t="s">
         <v>17</v>

</xml_diff>